<commit_message>
Increase the update_xl sleep time to 20 secondsm
Earlier sleep time of 2 seconds was not sufficient for the full URL to load thus the extracted coordinates were imprecise. Increasing the sleep time to 20 seconds gurantees that the exact exact coordinates extracted. 20 seconds is likely an overkill but the script only needs to be run once , so the additional delay is acceptable.
</commit_message>
<xml_diff>
--- a/data/cbus_trivia_list_updated.xlsx
+++ b/data/cbus_trivia_list_updated.xlsx
@@ -1302,7 +1302,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Daily+Growler+-+UA/@40.030734,-83.095906,1044m/data=!3m3!1e3!4b1!5s0x8838921a94156c4f:0xc7c5d0f7e3fffd0c!4m6!3m5!1s0x8838921a95481c21:0x8c0adb33c1c10db4!8m2!3d40.03073!4d-83.0910351!16s%2Fg%2F1hhjfc_tc?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Daily+Growler+-+UA/@40.03073,-83.0910351,548m/data=!3m3!1e3!4b1!5s0x8838921a94156c4f:0xc7c5d0f7e3fffd0c!4m6!3m5!1s0x8838921a95481c21:0x8c0adb33c1c10db4!8m2!3d40.03073!4d-83.0910351!16s%2Fg%2F1hhjfc_tc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G2" s="10" t="n"/>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Daily+Growler+-+UA/@40.030734,-83.095906,1044m/data=!3m3!1e3!4b1!5s0x8838921a94156c4f:0xc7c5d0f7e3fffd0c!4m6!3m5!1s0x8838921a95481c21:0x8c0adb33c1c10db4!8m2!3d40.03073!4d-83.0910351!16s%2Fg%2F1hhjfc_tc?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Daily+Growler+-+UA/@40.03073,-83.0910351,548m/data=!3m3!1e3!4b1!5s0x8838921a94156c4f:0xc7c5d0f7e3fffd0c!4m6!3m5!1s0x8838921a95481c21:0x8c0adb33c1c10db4!8m2!3d40.03073!4d-83.0910351!16s%2Fg%2F1hhjfc_tc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N2" s="10" t="n"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Daily+Growler+-+German+Village%2FBrewery+District/@39.9477427,-83.0001923,16z/data=!3m1!4b1!4m6!3m5!1s0x88388f4c3bf5b523:0x831882459195cf3f!8m2!3d39.9477386!4d-82.997612!16s%2Fg%2F11d_x4fh86?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Daily+Growler+-+German+Village%2FBrewery+District/@39.9477386,-82.997612,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f4c3bf5b523:0x831882459195cf3f!8m2!3d39.9477386!4d-82.997612!16s%2Fg%2F11d_x4fh86?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U2" s="10" t="n"/>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.0918628,-82.8537584,17z/data=!3m1!4b1!4m6!3m5!1s0x88385e265c7fe531:0xb6f8e2caba9375ec!8m2!3d40.0918587!4d-82.8511781!16s%2Fg%2F11btn1dy21?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.0918587,-82.8511781,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88385e265c7fe531:0xb6f8e2caba9375ec!8m2!3d40.0918587!4d-82.8511781!16s%2Fg%2F11btn1dy21?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB2" s="10" t="n"/>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572023,-83.0123703,15z/data=!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572023,-83.0123703,15z/data=!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI2" s="10" t="n"/>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Homefield:+Iconic+Sports+Bar/@39.9845191,-83.0470563,1053m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51a690bf95:0x39701495d80234e7!8m2!3d39.9845191!4d-83.0444814!16s%2Fg%2F11w4399plq?entry=tts&amp;g_ep=EgoyMDI0MTExOC4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Homefield:+Iconic+Sports+Bar/@39.9845191,-83.0444814,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51a690bf95:0x39701495d80234e7!8m2!3d39.9845191!4d-83.0444814!16s%2Fg%2F11w4399plq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G3" s="10" t="n"/>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Edison+Brewing+Company/@39.9973925,-82.8467394,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883863dda8e280e9:0x9f5172e7fc525537!8m2!3d39.9973884!4d-82.8441645!16s%2Fg%2F11jg2sp2ss?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Edison+Brewing+Company/@39.9973884,-82.8441645,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883863dda8e280e9:0x9f5172e7fc525537!8m2!3d39.9973884!4d-82.8441645!16s%2Fg%2F11jg2sp2ss?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N3" s="10" t="n"/>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/DraftKings+Sports+%26+Social+Columbus/@39.9795428,-83.0064367,933m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f0c9732fe45:0xe6466571e35a6f76!8m2!3d39.9795387!4d-83.0038618!16s%2Fg%2F11vw_x7zjs?entry=tts&amp;g_ep=EgoyMDI0MDkyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/DraftKings+Sports+%26+Social+Columbus/@39.9795387,-83.0038618,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f0c9732fe45:0xe6466571e35a6f76!8m2!3d39.9795387!4d-83.0038618!16s%2Fg%2F11vw_x7zjs?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U3" s="10" t="n"/>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.123482,-82.9859953,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f490ed9d9f63:0x62e80188ea19bc64!8m2!3d40.123478!4d-82.9811298!16s%2Fg%2F1tfjrcf6?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.123478,-82.9811298,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f490ed9d9f63:0x62e80188ea19bc64!8m2!3d40.123478!4d-82.9811298!16s%2Fg%2F1tfjrcf6?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB3" s="10" t="n"/>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Library+Bar/@40.0066411,-83.0121141,16z/data=!3m2!4b1!5s0x88388ea35408066f:0x39b3154da1495266!4m6!3m5!1s0x88388ea3566d0bc7:0xbe31a43f901b211f!8m2!3d40.006637!4d-83.0095338!16s%2Fg%2F1tgkhyzc?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Library+Bar/@40.006637,-83.0095338,548m/data=!3m3!1e3!4b1!5s0x88388ea35408066f:0x39b3154da1495266!4m6!3m5!1s0x88388ea3566d0bc7:0xbe31a43f901b211f!8m2!3d40.006637!4d-83.0095338!16s%2Fg%2F1tgkhyzc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G4" s="10" t="n"/>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Endeavor+Brewing+and+Spirits/@39.9879229,-83.0329628,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ef0ae6aad49:0xda62ac8e1f0affdc!8m2!3d39.9879188!4d-83.0303879!16s%2Fg%2F11f0y2pkz4?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Endeavor+Brewing+and+Spirits/@39.9879188,-83.0303879,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ef0ae6aad49:0xda62ac8e1f0affdc!8m2!3d39.9879188!4d-83.0303879!16s%2Fg%2F11f0y2pkz4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N4" s="10" t="n"/>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hamilton's+Pub/@40.0654651,-82.8643139,932m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883860f5cc689aaf:0x5a87f57f1cfded26!8m2!3d40.065461!4d-82.861739!16s%2Fg%2F1tx1tvv0?entry=tts&amp;g_ep=EgoyMDI0MDkyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hamilton's+Pub/@40.065461,-82.861739,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883860f5cc689aaf:0x5a87f57f1cfded26!8m2!3d40.065461!4d-82.861739!16s%2Fg%2F1tx1tvv0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U4" s="10" t="n"/>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Endeavor+Brewing+and+Spirits/@39.9879229,-83.0329682,17z/data=!3m1!4b1!4m6!3m5!1s0x88388ef0ae6aad49:0xda62ac8e1f0affdc!8m2!3d39.9879188!4d-83.0303879!16s%2Fg%2F11f0y2pkz4?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Endeavor+Brewing+and+Spirits/@39.9879188,-83.0303879,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ef0ae6aad49:0xda62ac8e1f0affdc!8m2!3d39.9879188!4d-83.0303879!16s%2Fg%2F11f0y2pkz4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB4" s="10" t="n"/>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Dalton+Union+Winery+%26+Brewery/@40.2968578,-83.4518898,17z/data=!3m1!4b1!4m6!3m5!1s0x8838d024b368ce67:0x4fc03e870739c146!8m2!3d40.2968537!4d-83.4493095!16s%2Fg%2F11bw61fl7y?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Dalton+Union+Winery+%26+Brewery/@40.2968537,-83.4493095,17z/data=!3m1!4b1!4m6!3m5!1s0x8838d024b368ce67:0x4fc03e870739c146!8m2!3d40.2968537!4d-83.4493095!16s%2Fg%2F11bw61fl7y?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI4" s="10" t="n"/>
@@ -1745,7 +1745,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Seventh+Son+Brewing+Co./@39.9853671,-83.0022751,16z/data=!3m1!4b1!4m6!3m5!1s0x88388ece1e570549:0x76d37b7748664e44!8m2!3d39.985363!4d-82.9996948!16s%2Fg%2F11r8kbv3_?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Seventh+Son+Brewing+Co./@39.985363,-82.9996948,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ece1e570549:0x76d37b7748664e44!8m2!3d39.985363!4d-82.9996948!16s%2Fg%2F11r8kbv3_?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G5" s="10" t="n"/>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Harry+Buffalo+Westerville/@40.0845723,-82.8971878,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838600f168a2c65:0x3192cb7ebd34470d!8m2!3d40.0845682!4d-82.8946129!16s%2Fg%2F11b6vghmry?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Harry+Buffalo+Westerville/@40.0845682,-82.8946129,1095m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838600f168a2c65:0x3192cb7ebd34470d!8m2!3d40.0845682!4d-82.8946129!16s%2Fg%2F11b6vghmry?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N5" s="10" t="n"/>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mainline+Bar+%2B+Courtyard/@39.9569527,-82.9984669,1036m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388fd404b48a7b:0x9921f72996e68dcd!8m2!3d39.9569487!4d-82.993596!16s%2Fg%2F11wr87hh3w?entry=tts&amp;g_ep=EgoyMDI1MDEwNy4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Mainline+Bar+%2B+Courtyard/@39.9569487,-82.993596,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388fd404b48a7b:0x9921f72996e68dcd!8m2!3d39.9569487!4d-82.993596!16s%2Fg%2F11wr87hh3w?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U5" s="10" t="n"/>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Dempsey's+Food+%26+Spirits/@39.9550422,-82.9989121,15z/data=!4m6!3m5!1s0x88388f3606695327:0x2b4b1aecbd9fcdc7!8m2!3d39.9550422!4d-82.9989121!16s%2Fg%2F11r8qypbp?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MDYyMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Dempsey's+Food+%26+Spirits/@39.9550422,-82.9989121,2195m/data=!3m1!1e3!4m6!3m5!1s0x88388f3606695327:0x2b4b1aecbd9fcdc7!8m2!3d39.9550422!4d-82.9989121!16s%2Fg%2F11r8qypbp?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB5" s="10" t="n"/>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Jackie+O's+On+Fourth/@39.9663521,-82.9971442,4210m/data=!3m1!1e3!4m6!3m5!1s0x88388f255810de45:0x89eb40454b3869d0!8m2!3d39.9663521!4d-82.9971442!16s%2Fg%2F11l7m0t2_r?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;cshid=1733161602185686&amp;entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Jackie+O's+On+Fourth/@39.9663521,-82.9971442,4389m/data=!3m1!1e3!4m6!3m5!1s0x88388f255810de45:0x89eb40454b3869d0!8m2!3d39.9663521!4d-82.9971442!16s%2Fg%2F11l7m0t2_r?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G6" s="10" t="n"/>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Lee's+Sports+%26+Spirits/@40.1073135,-83.2711028,1043m/data=!3m3!1e3!4b1!5s0x8838bff3973e2d9b:0x6413f9c65d6ad27a!4m6!3m5!1s0x8838bff39713427b:0x4d3e88482151642b!8m2!3d40.1073094!4d-83.2685279!16s%2Fg%2F1twy_6hg?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Lee's+Sports+%26+Spirits/@40.1073094,-83.2685279,1095m/data=!3m3!1e3!4b1!5s0x8838bff3973e2d9b:0x6413f9c65d6ad27a!4m6!3m5!1s0x8838bff39713427b:0x4d3e88482151642b!8m2!3d40.1073094!4d-83.2685279!16s%2Fg%2F1twy_6hg?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N6" s="10" t="n"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill+Crosswoods/@40.117811,-83.0155732,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f3403b873fd5:0xdcf9c2b33af3b50c!8m2!3d40.1178069!4d-83.0129929!16s%2Fg%2F11cn7syqct?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill+Crosswoods/@40.1178069,-83.0129929,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f3403b873fd5:0xdcf9c2b33af3b50c!8m2!3d40.1178069!4d-83.0129929!16s%2Fg%2F11cn7syqct?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U6" s="10" t="n"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Grizzlybird+Brewing+Company/@40.1543289,-82.9238861,299m/data=!3m1!1e3!4m6!3m5!1s0x883843abccfda7db:0xc2d6472030ade30f!8m2!3d40.1544914!4d-82.9233841!16s%2Fg%2F11gn0_lk74?entry=tts&amp;g_ep=EgoyMDI1MDEwNi4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Grizzlybird+Brewing+Company/@40.1543289,-82.9238861,547m/data=!3m1!1e3!4m6!3m5!1s0x883843abccfda7db:0xc2d6472030ade30f!8m2!3d40.1544914!4d-82.9233841!16s%2Fg%2F11gn0_lk74?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB6" s="10" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Global+Gallery+Coffee+Shop/@40.0341716,-83.019368,1012m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c3e50bce2e7:0x4fbf24edfdec3f44!8m2!3d40.0341716!4d-83.0167931!16s%2Fg%2F1tf7hb48?entry=tts&amp;g_ep=EgoyMDI1MDEyOS4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Global+Gallery+Coffee+Shop/@40.0341716,-83.0167931,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c3e50bce2e7:0x4fbf24edfdec3f44!8m2!3d40.0341716!4d-83.0167931!16s%2Fg%2F1tf7hb48?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI6" s="10" t="n"/>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Carfagna's+Ristorante/@40.1499236,-82.981462,17z/data=!3m2!4b1!5s0x8838f46e562ca469:0x2ef79b7345bc86c!4m6!3m5!1s0x8838f45abd40e6b3:0x69e05a11e1779fdf!8m2!3d40.1499195!4d-82.9788817!16s%2Fg%2F1tfgq1hs?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Carfagna's+Ristorante/@40.1499195,-82.9788817,547m/data=!3m3!1e3!4b1!5s0x8838f46e562ca469:0x2ef79b7345bc86c!4m6!3m5!1s0x8838f45abd40e6b3:0x69e05a11e1779fdf!8m2!3d40.1499195!4d-82.9788817!16s%2Fg%2F1tfgq1hs?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G7" s="10" t="n"/>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Porch+Growler/@40.0920425,-83.0201657,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388cc975c89c31:0xe35c49c3c47913dc!8m2!3d40.0920384!4d-83.0175908!16s%2Fg%2F11ghs9625m?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Porch+Growler/@40.0920384,-83.0175908,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388cc975c89c31:0xe35c49c3c47913dc!8m2!3d40.0920384!4d-83.0175908!16s%2Fg%2F11ghs9625m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N7" s="10" t="n"/>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+at+Grandview+Yard/@39.9747759,-83.0288768,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f616419a2bf:0x6e58cecfe2b5dfde!8m2!3d39.9747718!4d-83.0262965!16s%2Fg%2F11vlc5j42k?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+at+Grandview+Yard/@39.9747718,-83.0262965,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f616419a2bf:0x6e58cecfe2b5dfde!8m2!3d39.9747718!4d-83.0262965!16s%2Fg%2F11vlc5j42k?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U7" s="10" t="n"/>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mainline+Bar+%2B+Courtyard/@39.9569527,-82.9984669,1036m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388fd404b48a7b:0x9921f72996e68dcd!8m2!3d39.9569487!4d-82.993596!16s%2Fg%2F11wr87hh3w?entry=tts&amp;g_ep=EgoyMDI1MDEwNy4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Mainline+Bar+%2B+Courtyard/@39.9569487,-82.993596,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388fd404b48a7b:0x9921f72996e68dcd!8m2!3d39.9569487!4d-82.993596!16s%2Fg%2F11wr87hh3w?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB7" s="10" t="n"/>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+New+Albany/@40.0822237,-82.8134093,16z/data=!3m1!4b1!4m6!3m5!1s0x8838594eee81e151:0x7e8393e68e982a37!8m2!3d40.0822196!4d-82.810829!16s%2Fg%2F11px9wd66y?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/BrewDog+New+Albany/@40.0822196,-82.810829,1095m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838594eee81e151:0x7e8393e68e982a37!8m2!3d40.0822196!4d-82.810829!16s%2Fg%2F11px9wd66y?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G8" s="10" t="n"/>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Sweet+Harmony+Canal/@39.8426758,-82.8103307,1047m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387b31bb711887:0x8ad938223f5654f9!8m2!3d39.8426717!4d-82.8077558!16s%2Fg%2F11l5h7qrjv?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Sweet+Harmony+Canal/@39.8426717,-82.8077558,550m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387b31bb711887:0x8ad938223f5654f9!8m2!3d39.8426717!4d-82.8077558!16s%2Fg%2F11l5h7qrjv?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N8" s="10" t="n"/>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/World+of+Beer/@40.0492371,-82.9196833,17z/data=!3m1!4b1!4m6!3m5!1s0x88388a7d1fe1c23b:0xa62428c041be0e2a!8m2!3d40.049233!4d-82.917103!16s%2Fg%2F1hhkjqcmk?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/World+of+Beer/@40.049233,-82.917103,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388a7d1fe1c23b:0xa62428c041be0e2a!8m2!3d40.049233!4d-82.917103!16s%2Fg%2F1hhkjqcmk?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U8" s="10" t="n"/>
@@ -2244,7 +2244,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Adobe+Gilas/@40.0500842,-82.917909,17z/data=!3m1!4b1!4m6!3m5!1s0x88388a7d0e30b961:0x9f5912c1ccd07b52!8m2!3d40.0500801!4d-82.9153287!16s%2Fg%2F1tk_pykr?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Adobe+Gilas/@40.0500801,-82.9153287,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388a7d0e30b961:0x9f5912c1ccd07b52!8m2!3d40.0500801!4d-82.9153287!16s%2Fg%2F1tk_pykr?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB8" s="10" t="n"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Byrne's+Pub/@39.9850146,-83.041501,16z/data=!3m1!4b1!4m6!3m5!1s0x88388e57001288e1:0xd4c15a5f8359744d!8m2!3d39.9850105!4d-83.0389207!16s%2Fg%2F1tdk5vkn?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Byrne's+Pub/@39.9850105,-83.0389207,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e57001288e1:0xd4c15a5f8359744d!8m2!3d39.9850105!4d-83.0389207!16s%2Fg%2F1tdk5vkn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G9" s="10" t="n"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Walrus/@39.9563609,-82.9980225,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f350437711d:0x7807339e67bc22e2!8m2!3d39.9563609!4d-82.9954476!16s%2Fg%2F11b7wc4_c5?sca_esv=3571e5df92edb3af&amp;output=search&amp;q=the+walrus,+columbus&amp;source=lnms&amp;fbs=AEQNm0Aa4sjWe7Rqy32pFwRj0UkWd8nbOJfsBGGB5IQQO6L3J5fCQuDw5vrzPt_cVO2GgWUj9lYp6rkuKNKs7T0vX7Q81Ek5YpPyUVFe3W7KrgIFN0yr210hnrD8iUeaBLQnVQx6xj_2rK51OT45p2-pNecGYGnmKIXSx0uVV4QrbXN8rzF_OS7YkBBO-_3NzudI87-yS3TEd_g5PthVlYyBSDYpFG4Prg&amp;ved=1t:200715&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Walrus/@39.9563609,-82.9980225,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f350437711d:0x7807339e67bc22e2!8m2!3d39.9563609!4d-82.9954476!16s%2Fg%2F11b7wc4_c5?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N9" s="10" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Aficionado's/@40.152454,-82.995854,1010m/data=!3m1!1e3!4m6!3m5!1s0x8838f3890b9aa70d:0x2697bd20fa1dedd3!8m2!3d40.152454!4d-82.995854!16s%2Fg%2F12vtvkx0j?entry=tts&amp;g_ep=EgoyMDI1MDIwNS4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Aficionado's/@40.152454,-82.995854,1094m/data=!3m1!1e3!4m6!3m5!1s0x8838f3890b9aa70d:0x2697bd20fa1dedd3!8m2!3d40.152454!4d-82.995854!16s%2Fg%2F12vtvkx0j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U9" s="10" t="n"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Good+Night+John+Boy/@39.9809956,-83.0066203,17z/data=!3m2!4b1!5s0x88388eda08f578ad:0xdb8bbc732bbf2dc5!4m6!3m5!1s0x88388fff45043a4f:0x7df810980370acc3!8m2!3d39.9809915!4d-83.00404!16s%2Fg%2F11ksbc2hq2?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Good+Night+John+Boy/@39.9809915,-83.00404,548m/data=!3m3!1e3!4b1!5s0x88388eda08f578ad:0xdb8bbc732bbf2dc5!4m6!3m5!1s0x88388fff45043a4f:0x7df810980370acc3!8m2!3d39.9809915!4d-83.00404!16s%2Fg%2F11ksbc2hq2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB9" s="10" t="n"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1053m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1098m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G10" s="10" t="n"/>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Zaftig+Brewing+Co+%26+Taproom/@40.1060707,-83.0003169,2086m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f353f7748f85:0xb62eb0b3e65c97e5!8m2!3d40.1060666!4d-82.997742!16s%2Fg%2F1q2w14jcq?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Zaftig+Brewing+Co+%26+Taproom/@40.1060666,-82.997742,1095m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f353f7748f85:0xb62eb0b3e65c97e5!8m2!3d40.1060666!4d-82.997742!16s%2Fg%2F1q2w14jcq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N10" s="10" t="n"/>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/City+Tavern/@39.9772859,-83.0008422,17z/data=!4m6!3m5!1s0x88388ed681e0dcc9:0xbe14933cdf6bb15d!8m2!3d39.9772818!4d-82.9982619!16s%2Fg%2F11c5_222c8?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/City+Tavern/@39.9772859,-83.0008422,549m/data=!3m1!1e3!4m6!3m5!1s0x88388ed681e0dcc9:0xbe14933cdf6bb15d!8m2!3d39.9772818!4d-82.9982619!16s%2Fg%2F11c5_222c8?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U10" s="10" t="n"/>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Olentangy+River+Brewing+Company/@40.1554407,-83.0150282,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f395ceefffff:0xb4503eb1b1af7c54!8m2!3d40.1554366!4d-83.0124479!16s%2Fg%2F11hcn9qywl?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Olentangy+River+Brewing+Company/@40.1554366,-83.0124479,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f395ceefffff:0xb4503eb1b1af7c54!8m2!3d40.1554366!4d-83.0124479!16s%2Fg%2F11hcn9qywl?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB10" s="10" t="n"/>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Gatsby's/@40.0209565,-82.8691971,16z/data=!3m1!4b1!4m6!3m5!1s0x8838619c52bb009f:0xfc7eaa8c3eb1dc41!8m2!3d40.0209524!4d-82.8666168!16s%2Fg%2F1tfmjgvw?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Gatsby's/@40.0209524,-82.8666168,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838619c52bb009f:0xfc7eaa8c3eb1dc41!8m2!3d40.0209524!4d-82.8666168!16s%2Fg%2F1tfmjgvw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI10" s="10" t="n"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Keystone+Pub+%26+Patio+Lewis+Center/@40.2017115,-83.0289519,1063m/data=!3m3!1e3!4b1!5s0x8838f10d4faabe19:0x65d6111fd7015a5e!4m6!3m5!1s0x8838f12a8de9ae49:0xbc1357b428f524c!8m2!3d40.2017074!4d-83.026377!16s%2Fg%2F11fcv7qd4s?entry=tts&amp;g_ep=EgoyMDI0MTIwOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Keystone+Pub+%26+Patio+Lewis+Center/@40.2017074,-83.026377,547m/data=!3m3!1e3!4b1!5s0x8838f10d4faabe19:0x65d6111fd7015a5e!4m6!3m5!1s0x8838f12a8de9ae49:0xbc1357b428f524c!8m2!3d40.2017074!4d-83.026377!16s%2Fg%2F11fcv7qd4s?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G11" s="10" t="n"/>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Bada+Bean+Bada+Booze/@39.980466,-83.0004425,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f67b407c1a9:0x5557be4d7dfac7e7!8m2!3d39.9804619!4d-82.9978676!16s%2Fg%2F11sb_n85p2?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Bada+Bean+Bada+Booze/@39.9804619,-82.9978676,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f67b407c1a9:0x5557be4d7dfac7e7!8m2!3d39.9804619!4d-82.9978676!16s%2Fg%2F11sb_n85p2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N11" s="10" t="n"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ethyl+%26+Tank/@39.9976707,-83.009534,2089m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eb8fa03002b:0x4926e68f3519af71!8m2!3d39.9976666!4d-83.0069591!16s%2Fg%2F11b6dqbnk5?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Ethyl+%26+Tank/@39.9976666,-83.0069591,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eb8fa03002b:0x4926e68f3519af71!8m2!3d39.9976666!4d-83.0069591!16s%2Fg%2F11b6dqbnk5?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U11" s="10" t="n"/>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Park+Street+Tavern/@39.9723411,-83.0073524,16z/data=!3m1!4b1!4m6!3m5!1s0x88388f26319fdc49:0xa156a7e175f440c0!8m2!3d39.972337!4d-83.0047721!16s%2Fm%2F0kffvcq?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Park+Street+Tavern/@39.972337,-83.0047721,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f26319fdc49:0xa156a7e175f440c0!8m2!3d39.972337!4d-83.0047721!16s%2Fm%2F0kffvcq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB11" s="10" t="n"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Traditions+Tavern/@40.0513417,-83.0518852,16z/data=!3m1!4b1!4m6!3m5!1s0x88388da51cf8b497:0x8427d832e5436760!8m2!3d40.0513376!4d-83.0493049!16s%2Fg%2F1td6n9x4?entry=tts&amp;g_ep=EgoyMDI0MDYwNS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Traditions+Tavern/@40.0513376,-83.0493049,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388da51cf8b497:0x8427d832e5436760!8m2!3d40.0513376!4d-83.0493049!16s%2Fg%2F1td6n9x4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G12" s="10" t="n"/>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Bobcat+Sports+Bar/@39.9795836,-83.03383,1013m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f8b1d3ff009:0xa4dca0a665e815f6!8m2!3d39.9795836!4d-83.03383!16s%2Fg%2F11k9h02cd_?entry=tts&amp;g_ep=EgoyMDI1MDIwNS4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Bobcat+Sports+Bar/@39.9795836,-83.03383,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f8b1d3ff009:0xa4dca0a665e815f6!8m2!3d39.9795836!4d-83.03383!16s%2Fg%2F11k9h02cd_?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N12" s="10" t="n"/>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hank's+Texas+BBQ/@40.0221281,-83.0163303,17z/data=!3m1!4b1!4m6!3m5!1s0x88388dc36b1f1fdb:0x3a5f374dc427ef9a!8m2!3d40.022124!4d-83.01375!16s%2Fg%2F11ngs94fmg?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Hank's+Texas+BBQ/@40.022124,-83.01375,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388dc36b1f1fdb:0x3a5f374dc427ef9a!8m2!3d40.022124!4d-83.01375!16s%2Fg%2F11ngs94fmg?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U12" s="10" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Rule+3/@39.9030536,-82.7796096,16z/data=!3m1!4b1!4m6!3m5!1s0x88387b20bf2a71b3:0x357d7f0b307eb309!8m2!3d39.9030495!4d-82.7770293!16s%2Fg%2F1tg_b4ck?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Rule+3/@39.9030495,-82.7770293,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387b20bf2a71b3:0x357d7f0b307eb309!8m2!3d39.9030495!4d-82.7770293!16s%2Fg%2F1tg_b4ck?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB12" s="10" t="n"/>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Draft+Room/@40.1115233,-82.9483025,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f52171949c77:0x6ef99bfabccd0e0b!8m2!3d40.1115192!4d-82.9457222!16s%2Fg%2F11fy_59s1s?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Draft+Room/@40.1115192,-82.9457222,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f52171949c77:0x6ef99bfabccd0e0b!8m2!3d40.1115192!4d-82.9457222!16s%2Fg%2F11fy_59s1s?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI12" s="10" t="n"/>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Budd+Dairy+Food+Hall/@39.9851913,-83.0015041,1045m/data=!3m2!1e3!5s0x88388ece01f8c2b3:0x59527ee22e9e888a!4m6!3m5!1s0x88388ed1fd67ce55:0xd55d392b50a4f2c1!8m2!3d39.9851708!4d-82.9990111!16s%2Fg%2F11c56rj2y_?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Budd+Dairy+Food+Hall/@39.9851913,-83.0015041,1097m/data=!3m2!1e3!5s0x88388ece01f8c2b3:0x59527ee22e9e888a!4m6!3m5!1s0x88388ed1fd67ce55:0xd55d392b50a4f2c1!8m2!3d39.9851708!4d-82.9990111!16s%2Fg%2F11c56rj2y_?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N13" s="10" t="n"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Jac+%26+Do's+on+High/@39.9948996,-83.007562,111m/data=!3m1!1e3!4m6!3m5!1s0x88388f003ab47da7:0xd9b3a15e41257898!8m2!3d39.9948991!4d-83.0072908!16s%2Fg%2F11wptbkfz0?entry=tts&amp;g_ep=EgoyMDI0MTExOC4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Jac+%26+Do's+on+High/@39.9948996,-83.007562,137m/data=!3m1!1e3!4m6!3m5!1s0x88388f003ab47da7:0xd9b3a15e41257898!8m2!3d39.9948991!4d-83.0072908!16s%2Fg%2F11wptbkfz0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U13" s="10" t="n"/>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Slammers/@39.9658369,-82.9982074,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f2d7502487f:0xb1fea5f6dc7ee8a2!8m2!3d39.9658328!4d-82.9956271!16s%2Fg%2F1td3s4q0?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Slammers/@39.9658328,-82.9956271,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f2d7502487f:0xb1fea5f6dc7ee8a2!8m2!3d39.9658328!4d-82.9956271!16s%2Fg%2F1td3s4q0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB13" s="10" t="n"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Fenders/@40.1350976,-82.9891967,4170m/data=!3m1!1e3!4m6!3m5!1s0x8838f480d8b4a5ad:0x11f9631be0916186!8m2!3d40.1350976!4d-82.9891967!16s%2Fg%2F1260b39s2?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Fenders/@40.1350976,-82.9891967,4378m/data=!3m1!1e3!4m6!3m5!1s0x8838f480d8b4a5ad:0x11f9631be0916186!8m2!3d40.1350976!4d-82.9891967!16s%2Fg%2F1260b39s2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N14" s="10" t="n"/>
@@ -3052,7 +3052,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Level+One+Bar+%2B+Arcade/@40.1146905,-83.0137412,16z/data=!3m1!4b1!4m6!3m5!1s0x8838f340cc8c1325:0x4a514f2124d979b0!8m2!3d40.1146864!4d-83.0111609!16s%2Fg%2F11bw2j_5x8?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Level+One+Bar+%2B+Arcade/@40.1146864,-83.0111609,1095m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f340cc8c1325:0x4a514f2124d979b0!8m2!3d40.1146864!4d-83.0111609!16s%2Fg%2F11bw2j_5x8?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U14" s="10" t="n"/>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Zeno's/@39.9840557,-83.0178853,17z/data=!3m1!4b1!4m6!3m5!1s0x88388ee783536759:0xc84ea701e7b579ac!8m2!3d39.9840516!4d-83.015305!16s%2Fg%2F1trrdw5w?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Zeno's/@39.9840516,-83.015305,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ee783536759:0xc84ea701e7b579ac!8m2!3d39.9840516!4d-83.015305!16s%2Fg%2F1trrdw5w?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB14" s="10" t="n"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/India+Oak+Grill/@40.03315,-83.0025291,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c0c5c53c593:0x17c7304ffff74fed!8m2!3d40.0331459!4d-82.9999542!16s%2Fg%2F1xg5tbg0?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/India+Oak+Grill/@40.0331459,-82.9999542,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c0c5c53c593:0x17c7304ffff74fed!8m2!3d40.0331459!4d-82.9999542!16s%2Fg%2F1xg5tbg0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N15" s="10" t="n"/>
@@ -3160,7 +3160,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pierogi+Mountain/@39.9655682,-82.9945033,17z/data=!3m1!4b1!4m6!3m5!1s0x88388eaef3e0849f:0xa5c30c0dcaadeedf!8m2!3d39.9655641!4d-82.991923!16s%2Fg%2F11bx1yvh_q?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pierogi+Mountain/@39.9655641,-82.991923,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eaef3e0849f:0xa5c30c0dcaadeedf!8m2!3d39.9655641!4d-82.991923!16s%2Fg%2F11bx1yvh_q?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U15" s="10" t="n"/>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/840+Lounge/@39.9728238,-82.8995711,4209m/data=!3m1!1e3!4m6!3m5!1s0x8838627c679bb7a3:0xc0e9a01727adbbe9!8m2!3d39.9728238!4d-82.8995711!16s%2Fg%2F1tcxkf87?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/840+Lounge/@39.9728238,-82.8995711,4388m/data=!3m1!1e3!4m6!3m5!1s0x8838627c679bb7a3:0xc0e9a01727adbbe9!8m2!3d39.9728238!4d-82.8995711!16s%2Fg%2F1tcxkf87?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB15" s="10" t="n"/>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ledo's+Tavern/@40.0155031,-83.0139529,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ea08c8fb9bd:0x2462991b2fec2a0d!8m2!3d40.015499!4d-83.011378!16s%2Fg%2F1tqclwrq?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Ledo's+Tavern/@40.015499,-83.011378,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ea08c8fb9bd:0x2462991b2fec2a0d!8m2!3d40.015499!4d-83.011378!16s%2Fg%2F1tqclwrq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N16" s="10" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Railhouse/@39.9624978,-82.9601736,17z/data=!3m1!4b1!4m6!3m5!1s0x8838898413cc993b:0xb2c1418c3640673e!8m2!3d39.9624937!4d-82.9575933!16s%2Fg%2F11sg_fd1k5?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Railhouse/@39.9624937,-82.9575933,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838898413cc993b:0xb2c1418c3640673e!8m2!3d39.9624937!4d-82.9575933!16s%2Fg%2F11sg_fd1k5?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U16" s="10" t="n"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/O'Nelly's+Sports+Pub+%26+Grill/@40.1517825,-83.000682,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f38915ab0801:0xcff7ad999275fde2!8m2!3d40.1517785!4d-82.9958165!16s%2Fg%2F12hn96vlw?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/O'Nelly's+Sports+Pub+%26+Grill/@40.1517785,-82.9958165,1094m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f38915ab0801:0xcff7ad999275fde2!8m2!3d40.1517785!4d-82.9958165!16s%2Fg%2F12hn96vlw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB16" s="10" t="n"/>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="AH16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+Short+North/@39.9863181,-83.0081128,17z/data=!3m1!4b1!4m6!3m5!1s0x88388ec53a33fe95:0x974490f6f707d0e3!8m2!3d39.986314!4d-83.0055325!16s%2Fg%2F11hcw4dg65?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/BrewDog+Short+North/@39.986314,-83.0055325,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec53a33fe95:0x974490f6f707d0e3!8m2!3d39.986314!4d-83.0055325!16s%2Fg%2F11hcw4dg65?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI16" s="10" t="n"/>
@@ -3394,7 +3394,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Seek-No-Further+Cidery/@40.0671359,-82.5219815,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838159544e31333:0x416acad79b2ab08e!8m2!3d40.0671318!4d-82.5194066!16s%2Fg%2F11nnvhf7s3?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Seek-No-Further+Cidery/@40.0671318,-82.5194066,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838159544e31333:0x416acad79b2ab08e!8m2!3d40.0671318!4d-82.5194066!16s%2Fg%2F11nnvhf7s3?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N17" s="10" t="n"/>
@@ -3423,7 +3423,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Saucy+Brew+Works+-+Columbus/@39.9838158,-83.0195792,17z/data=!3m2!4b1!5s0x88388ee7aa146b73:0xcaf6f4a62ccded0e!4m6!3m5!1s0x88388f6efb8530ad:0xb272da1027952abb!8m2!3d39.9838117!4d-83.0169989!16s%2Fg%2F11fwj9l2s9?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Saucy+Brew+Works+Columbus+-+Brewpub+%26+Coffeehouse/@39.9838117,-83.0169989,1097m/data=!3m3!1e3!4b1!5s0x88388ee7aa146b73:0xcaf6f4a62ccded0e!4m6!3m5!1s0x88388f6efb8530ad:0xb272da1027952abb!8m2!3d39.9838117!4d-83.0169989!16s%2Fg%2F11fwj9l2s9?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U17" s="10" t="n"/>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Submarine+House/@39.9880693,-83.0468766,15z/data=!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Submarine+House/@39.9880693,-83.0468766,2194m/data=!3m1!1e3!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB17" s="10" t="n"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Fourth+Street+Taproom+%26+Kitchen/@40.0003488,-83.0009686,17z/data=!3m1!4b1!4m6!3m5!1s0x88388eb4011d028f:0x1394833d995b526!8m2!3d40.0003447!4d-82.9983883!16s%2Fg%2F1tksp0f6?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Fourth+Street+Taproom+%26+Kitchen/@40.0003447,-82.9983883,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eb4011d028f:0x1394833d995b526!8m2!3d40.0003447!4d-82.9983883!16s%2Fg%2F1tksp0f6?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI17" s="10" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Uncle+Johnnie%E2%80%99s/@40.1527018,-82.686603,1042m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883843006d8f38cb:0x4bd7a7b96d6449a3!8m2!3d40.1526977!4d-82.6840281!16s%2Fg%2F11y2krc8s2?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Uncle+Johnnie%E2%80%99s/@40.1526977,-82.6840281,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883843006d8f38cb:0x4bd7a7b96d6449a3!8m2!3d40.1526977!4d-82.6840281!16s%2Fg%2F11y2krc8s2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N18" s="10" t="n"/>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Time+%26+Change/@40.132389,-82.8898445,17z/data=!3m1!4b1!4m6!3m5!1s0x88385f0aaa752acf:0x7b0587e826c2c009!8m2!3d40.1323849!4d-82.8872642!16s%2Fg%2F1tg4xhpr?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Time+%26+Change+-+Neighborhood+Gathering+Place/@40.1323849,-82.8872642,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88385f0aaa752acf:0x7b0587e826c2c009!8m2!3d40.1323849!4d-82.8872642!16s%2Fg%2F1tg4xhpr?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U18" s="10" t="n"/>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Understory/@40.0144299,-83.0167538,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f3649678e7f:0xf4aee1174636270e!8m2!3d40.0144258!4d-83.0141735!16s%2Fg%2F11rgw95h97?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Understory/@40.0144258,-83.0141735,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3649678e7f:0xf4aee1174636270e!8m2!3d40.0144258!4d-83.0141735!16s%2Fg%2F11rgw95h97?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB18" s="10" t="n"/>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="AH18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Brew-Stirs+Beechwold+Tavern/@40.0631855,-83.0204606,1051m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d90f5bdbcd1:0x7189adc02d21ec2a!8m2!3d40.0631814!4d-83.0178857!16s%2Fg%2F11ql6f97sq?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Brew-Stirs+Beechwold+Tavern/@40.0631814,-83.0178857,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d90f5bdbcd1:0x7189adc02d21ec2a!8m2!3d40.0631814!4d-83.0178857!16s%2Fg%2F11ql6f97sq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI18" s="10" t="n"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Village+Idiot/@39.9916759,-83.0066832,2025m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec661f8920d:0x422300be0b0a8a5d!8m2!3d39.9916759!4d-83.0066832!16s%2Fg%2F1vqthfx8?authuser=0&amp;entry=tts&amp;g_ep=EgoyMDI1MDIwNS4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Village+Idiot/@39.9916759,-83.0066832,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec661f8920d:0x422300be0b0a8a5d!8m2!3d39.9916759!4d-83.0066832!16s%2Fg%2F1vqthfx8?authuser=0&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N19" s="10" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Vic+Village+Tavern/@39.9871964,-83.01506,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f99c3b3d8e1:0xd450f2c7a04cf093!8m2!3d39.9871923!4d-83.0124797!16s%2Fg%2F11tsfynpk7?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Vic+Village+Tavern/@39.9871923,-83.0124797,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f99c3b3d8e1:0xd450f2c7a04cf093!8m2!3d39.9871923!4d-83.0124797!16s%2Fg%2F11tsfynpk7?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U19" s="57" t="n"/>
@@ -3710,7 +3710,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Happenstance+Brewing+Project/@40.2376894,-83.3651099,1048m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838c5d7700748af:0x71b60ce4af0ec656!8m2!3d40.2376853!4d-83.362535!16s%2Fg%2F11ldkhr085?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Happenstance+Brewing+Project/@40.2376853,-83.362535,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838c5d7700748af:0x71b60ce4af0ec656!8m2!3d40.2376853!4d-83.362535!16s%2Fg%2F11ldkhr085?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB19" s="57" t="n"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="AH19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Daily+Bar/@39.9811264,-83.0015628,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f43c5cefb05:0x4cf6669b687ea03a!8m2!3d39.9811223!4d-82.9989825!16s%2Fg%2F11rd8_vpj4?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Daily+Bar/@39.9811223,-82.9989825,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f43c5cefb05:0x4cf6669b687ea03a!8m2!3d39.9811223!4d-82.9989825!16s%2Fg%2F11rd8_vpj4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI19" s="57" t="n"/>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Goat+Dublin/@40.0620176,-83.1759748,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838947b7bbbeafb:0x909c13072f12da01!8m2!3d40.0620135!4d-83.1733999!16s%2Fg%2F1tdnfy3x?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Goat+Dublin/@40.0620135,-83.1733999,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838947b7bbbeafb:0x909c13072f12da01!8m2!3d40.0620135!4d-83.1733999!16s%2Fg%2F1tdnfy3x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N20" s="10" t="n"/>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Yellow+Springs+Brewery+Taproom+%26+Kitchen/@39.9880693,-83.0468766,4212m/data=!3m2!1e3!5s0x88388c0490d1f293:0x7f7d8bcea8a16fb!4m6!3m5!1s0x88388d78793b1de7:0xd31edb4b5a2ad7a!8m2!3d40.0218129!4d-83.0022913!16s%2Fg%2F11l22jl97f?entry=tts&amp;g_ep=EgoyMDI0MTExOC4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Yellow+Springs+Brewery+Taproom+%26+Kitchen/@39.9880693,-83.0468766,4387m/data=!3m2!1e3!5s0x88388c0490d1f293:0x7f7d8bcea8a16fb!4m6!3m5!1s0x88388d78793b1de7:0xd31edb4b5a2ad7a!8m2!3d40.0218129!4d-83.0022913!16s%2Fg%2F11l22jl97f?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U20" s="57" t="n"/>
@@ -3832,7 +3832,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Brew-Stirs+on+23/@40.0757051,-83.1287743,24741m/data=!3m1!1e3!4m6!3m5!1s0x8838f373618cb14f:0x11ad2d78ed6832be!8m2!3d40.1341491!4d-83.0131269!16s%2Fg%2F1ptvs5ppn?entry=tts&amp;g_ep=EgoyMDI1MDIyNi4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Brew-Stirs+on+23/@40.0757051,-83.1287743,35054m/data=!3m1!1e3!4m6!3m5!1s0x8838f373618cb14f:0x11ad2d78ed6832be!8m2!3d40.1341491!4d-83.0131269!16s%2Fg%2F1ptvs5ppn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB20" s="57" t="n"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Clintonville)/@40.0225093,-83.0167083,17z/data=!3m1!4b1!4m6!3m5!1s0x88388d4171aff8a3:0x7c54608c8c482af9!8m2!3d40.0225052!4d-83.014128!16s%2Fg%2F11t7d4d5nw?entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Clintonville)/@40.0225052,-83.014128,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d4171aff8a3:0x7c54608c8c482af9!8m2!3d40.0225052!4d-83.014128!16s%2Fg%2F11t7d4d5nw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI20" s="57" t="n"/>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Goat+Gahanna/@40.0608201,-82.8512152,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883860ef20b68627:0xb1b6efb131fbf921!8m2!3d40.060816!4d-82.8486403!16s%2Fg%2F1tfb2nrf?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Goat+Gahanna/@40.060816,-82.8486403,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883860ef20b68627:0xb1b6efb131fbf921!8m2!3d40.060816!4d-82.8486403!16s%2Fg%2F1tfb2nrf?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N21" s="10" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Echo+Spirits+Distilling+Co./@39.988908,-83.0375969,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f4b17d3769b:0x336bfaed8059f751!8m2!3d39.988904!4d-83.032726!16s%2Fg%2F11h2fwjvnw?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Echo+Spirits+Distilling+Co./@39.9890068,-83.0327863,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f4b17d3769b:0x336bfaed8059f751!8m2!3d39.9890068!4d-83.0327863!16s%2Fg%2F11h2fwjvnw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U21" s="57" t="n"/>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Donerick's+Pub/@40.0691868,-83.0221326,16z/data=!3m1!4b1!4m6!3m5!1s0x88388cede6f00ccb:0x72276dfd5ec38a18!8m2!3d40.0691827!4d-83.0195523!16s%2Fg%2F11dxc1v5cz?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Donerick's+Pub/@40.0691827,-83.0195523,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388cede6f00ccb:0x72276dfd5ec38a18!8m2!3d40.0691827!4d-83.0195523!16s%2Fg%2F11dxc1v5cz?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB21" s="57" t="n"/>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="AH21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Gem%C3%BCt+Biergarten/@39.9633726,-82.9834169,17z/data=!3m1!4b1!4m6!3m5!1s0x883889b1d1a5cc8d:0xa948edf5d8fb4a31!8m2!3d39.9633685!4d-82.9808366!16s%2Fg%2F11ghpypvrb?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Gem%C3%BCt+Biergarten/@39.9633685,-82.9808366,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889b1d1a5cc8d:0xa948edf5d8fb4a31!8m2!3d39.9633685!4d-82.9808366!16s%2Fg%2F11ghpypvrb?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI21" s="57" t="n"/>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Goat+RiverSouth/@39.9576066,-83.0025739,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f368d224e33:0xb8ba98576f622440!8m2!3d39.9576025!4d-82.999999!16s%2Fg%2F11f3xwp6_m?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Goat+RiverSouth/@39.9576025,-82.999999,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f368d224e33:0xb8ba98576f622440!8m2!3d39.9576025!4d-82.999999!16s%2Fg%2F11f3xwp6_m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N22" s="57" t="n"/>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Gem%C3%BCt+Biergarten/@39.9633726,-82.9834169,17z/data=!3m1!4b1!4m6!3m5!1s0x883889b1d1a5cc8d:0xa948edf5d8fb4a31!8m2!3d39.9633685!4d-82.9808366!16s%2Fg%2F11ghpypvrb?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Gem%C3%BCt+Biergarten/@39.9633685,-82.9808366,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889b1d1a5cc8d:0xa948edf5d8fb4a31!8m2!3d39.9633685!4d-82.9808366!16s%2Fg%2F11ghpypvrb?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U22" s="57" t="n"/>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hop+Yard+62/@39.8816514,-83.0969185,17z/data=!3m1!4b1!4m6!3m5!1s0x88389b3938cee8f5:0x4c72cf03cafe710e!8m2!3d39.8816473!4d-83.0943382!16s%2Fg%2F11b727rljk?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Hop+Yard+62/@39.8816473,-83.0943382,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389b3938cee8f5:0x4c72cf03cafe710e!8m2!3d39.8816473!4d-83.0943382!16s%2Fg%2F11b727rljk?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB22" s="57" t="n"/>
@@ -4117,7 +4117,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/North+Market+Bridge+Park/@40.1042138,-83.1123283,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838eddf5cae392b:0xee8ed679ae6156aa!8m2!3d40.1042097!4d-83.1097534!16s%2Fg%2F11jq2c2qb7?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/North+Market+Bridge+Park/@40.1042097,-83.1097534,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838eddf5cae392b:0xee8ed679ae6156aa!8m2!3d40.1042097!4d-83.1097534!16s%2Fg%2F11jq2c2qb7?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N23" s="57" t="n"/>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Local+Cantina+-+Clintonville/@40.025905,-83.0166349,16z/data=!3m1!4b1!4m6!3m5!1s0x88388c180bf51e4d:0x1a9689e6396c477e!8m2!3d40.0259009!4d-83.0140546!16s%2Fg%2F11b6pwcz24?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Local+Cantina+-+Clintonville/@40.0259009,-83.0140546,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c180bf51e4d:0x1a9689e6396c477e!8m2!3d40.0259009!4d-83.0140546!16s%2Fg%2F11b6pwcz24?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U23" s="57" t="n"/>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Loose+Rail+Brewing/@39.8432622,-82.8095877,1047m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387be3ae072d43:0x52bb8cac97811b34!8m2!3d39.8432581!4d-82.8070128!16s%2Fg%2F11cssq40xw?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Loose+Rail+Brewing/@39.8432581,-82.8070128,550m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387be3ae072d43:0x52bb8cac97811b34!8m2!3d39.8432581!4d-82.8070128!16s%2Fg%2F11cssq40xw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB23" s="57" t="n"/>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mulligan's+Sports+Pub/@40.1180201,-83.0660705,3a,90y,349.39h,100.94t/data=!4m6!3m5!1s0x8838f28520d0886d:0xc5b211a57f97acb!8m2!3d40.1349429!4d-83.0717844!16s%2Fg%2F1th7y_w1?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Mulligan's+Sports+Pub/@40.1185137,-83.0661914,0m/data=!3m1!1e3!4m6!3m5!1s0x8838f28520d0886d:0xc5b211a57f97acb!8m2!3d40.1349429!4d-83.0717844!16s%2Fg%2F1th7y_w1?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N24" s="57" t="n"/>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mid+City+Garage/@39.9386603,-82.9935735,17z/data=!3m1!4b1!4m6!3m5!1s0x8838890042685bff:0xaa51efd0d2f25e8b!8m2!3d39.9386562!4d-82.9909932!16s%2Fg%2F11vq4__d66?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Mid+City+Garage/@39.9386553,-82.99099,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889771aed801b:0x5b79881f52ce2dc7!8m2!3d39.9386553!4d-82.99099!16s%2Fg%2F11j5k_spt4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U24" s="57" t="n"/>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Outerbelt+Brewing+%26+Taproom/@39.9438443,-82.9017181,106416m/data=!3m1!1e3!4m6!3m5!1s0x8838772ae06bcd69:0x78dc511920f97570!8m2!3d39.7602032!4d-82.6664589!16s%2Fg%2F11g2r6jhny?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Outerbelt+Brewing+%26+Taproom/@39.9438443,-82.9017181,140488m/data=!3m1!1e3!4m6!3m5!1s0x8838772ae06bcd69:0x78dc511920f97570!8m2!3d39.7602032!4d-82.6664589!16s%2Fg%2F11g2r6jhny?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB24" s="57" t="n"/>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Nasty's+Sports+Bar+%26+Restaurant/@40.0180869,-83.1399475,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838916465e4f523:0x39883e3f377c84c5!8m2!3d40.0180828!4d-83.1373726!16s%2Fg%2F126352pts?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Nasty's+Sports+Bar+%26+Restaurant/@40.0180828,-83.1373726,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838916465e4f523:0x39883e3f377c84c5!8m2!3d40.0180828!4d-83.1373726!16s%2Fg%2F126352pts?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N25" s="57" t="n"/>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Buffalo+Wild+Wings/@39.9964772,-83.0283783,14.63z/data=!4m7!3m6!1s0x88388ea3555d5397:0x1f83030bafcb1f6a!8m2!3d40.0062196!4d-83.0096581!15sCh1CdWZmYWxvIFdpbGQgV2luZ3Mgb2hpbyBzdGF0ZSIDiAEBWh8iHWJ1ZmZhbG8gd2lsZCB3aW5ncyBvaGlvIHN0YXRlkgEYY2hpY2tlbl93aW5nc19yZXN0YXVyYW504AEA!16s%2Fg%2F1tfzsl83?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Buffalo+Wild+Wings/@39.9964772,-83.0283783,4387m/data=!3m1!1e3!4m6!3m5!1s0x88388ea3555d5397:0x1f83030bafcb1f6a!8m2!3d40.0062196!4d-83.0096581!16s%2Fg%2F1tfzsl83?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U25" s="57" t="n"/>
@@ -4364,7 +4364,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beer+Barrel+Pizza+and+Grill/@40.0519301,-82.923112,17z/data=!3m1!4b1!4m6!3m5!1s0x88388be37fc4060f:0x39e85a931e08cdb0!8m2!3d40.051926!4d-82.9205317!16s%2Fg%2F11gr63z9t8?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Beer+Barrel+Pizza+%26+Grill/@40.051926,-82.9205317,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388be37fc4060f:0x39e85a931e08cdb0!8m2!3d40.051926!4d-82.9205317!16s%2Fg%2F11gr63z9t8?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB25" s="57" t="n"/>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Submarine+House/@40.0011271,-83.1586011,17z/data=!3m1!4b1!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Submarine+House/@40.001123,-83.1560208,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N26" s="57" t="n"/>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Blu-Willy%E2%80%99s/@39.8829843,-83.0959047,17z/data=!3m1!4b1!4m6!3m5!1s0x88389b2e5386332d:0x73b1bf78d5a62cdd!8m2!3d39.8829802!4d-83.0933244!16s%2Fg%2F11h_zrxngn?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Blu-Willy%E2%80%99s/@39.8829802,-83.0933244,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389b2e5386332d:0x73b1bf78d5a62cdd!8m2!3d39.8829802!4d-83.0933244!16s%2Fg%2F11h_zrxngn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U26" s="57" t="n"/>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Donerick's+Pub/@40.1174899,-82.9895691,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f498c99c3ab9:0x17da88ac291bfe5e!8m2!3d40.1174858!4d-82.9869888!16s%2Fg%2F1tfrslcb?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Donerick's+Pub/@40.1174858,-82.9869888,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f498c99c3ab9:0x17da88ac291bfe5e!8m2!3d40.1174858!4d-82.9869888!16s%2Fg%2F1tfrslcb?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB26" s="57" t="n"/>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hale%E2%80%99s+Ale+%26+Kitchen/@40.0289242,-83.1216094,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838922c607c7b7b:0xd20f77b84f628c6d!8m2!3d40.0289201!4d-83.1190345!16s%2Fg%2F11bbwnn7f0?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hale%E2%80%99s+Ale+%26+Kitchen/@40.0289201,-83.1190345,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838922c607c7b7b:0xd20f77b84f628c6d!8m2!3d40.0289201!4d-83.1190345!16s%2Fg%2F11bbwnn7f0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N27" s="57" t="n"/>
@@ -4535,7 +4535,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mulligan's+Sports+Pub/@40.1180201,-83.0660705,3a,90y,349.39h,100.94t/data=!4m6!3m5!1s0x8838f28520d0886d:0xc5b211a57f97acb!8m2!3d40.1349429!4d-83.0717844!16s%2Fg%2F1th7y_w1?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Mulligan's+Sports+Pub/@40.1185137,-83.0661914,0m/data=!3m1!1e3!4m6!3m5!1s0x8838f28520d0886d:0xc5b211a57f97acb!8m2!3d40.1349429!4d-83.0717844!16s%2Fg%2F1th7y_w1?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U27" s="57" t="n"/>
@@ -4560,7 +4560,7 @@
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Lazy+Chameleon/@40.1492524,-83.0941259,16z/data=!3m1!4b1!4m6!3m5!1s0x8838ed9ca3e110e3:0x197a57473cdc346d!8m2!3d40.1492483!4d-83.0915456!16s%2Fg%2F11xd7mj1r?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Lazy+Chameleon/@40.1492483,-83.0915456,1094m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838ed9ca3e110e3:0x197a57473cdc346d!8m2!3d40.1492483!4d-83.0915456!16s%2Fg%2F11xd7mj1r?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB27" s="57" t="n"/>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.0918628,-82.8537584,17z/data=!3m1!4b1!4m6!3m5!1s0x88385e265c7fe531:0xb6f8e2caba9375ec!8m2!3d40.0918587!4d-82.8511781!16s%2Fg%2F11btn1dy21?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.0918587,-82.8511781,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88385e265c7fe531:0xb6f8e2caba9375ec!8m2!3d40.0918587!4d-82.8511781!16s%2Fg%2F11btn1dy21?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N28" s="57" t="n"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Submarine+House/@39.9880693,-83.0468766,15z/data=!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Submarine+House/@39.9880693,-83.0468766,2194m/data=!3m1!1e3!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U28" s="57" t="n"/>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.9893291,-83.055563,16z/data=!3m1!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB28" s="57" t="n"/>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill+Crosswoods/@40.117811,-83.0155732,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f3403b873fd5:0xdcf9c2b33af3b50c!8m2!3d40.1178069!4d-83.0129929!16s%2Fg%2F11cn7syqct?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill+Crosswoods/@40.1178069,-83.0129929,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f3403b873fd5:0xdcf9c2b33af3b50c!8m2!3d40.1178069!4d-83.0129929!16s%2Fg%2F11cn7syqct?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N29" s="57" t="n"/>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Wolf's+Ridge+Brewing+-+Taproom/@39.9673419,-83.000014,1087m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f2c32a60e2b:0x24b903e1e0d50656!8m2!3d39.9673378!4d-82.9974391!16s%2Fg%2F11cm0h1zv6?entry=tts&amp;g_ep=EgoyMDI1MDIyNi4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Wolf's+Ridge+Brewing+-+Taproom/@39.9673378,-82.9974391,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f2c32a60e2b:0x24b903e1e0d50656!8m2!3d39.9673378!4d-82.9974391!16s%2Fg%2F11cm0h1zv6?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U29" s="57" t="n"/>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577654,-83.0140063,16z/data=!3m1!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB29" s="57" t="n"/>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+New+Albany/@40.0632073,-82.9581632,39329m/data=!3m1!1e3!4m6!3m5!1s0x8838594eee81e151:0x7e8393e68e982a37!8m2!3d40.0822196!4d-82.810829!16s%2Fg%2F11px9wd66y?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/BrewDog+New+Albany/@40.0632073,-82.9581632,70121m/data=!3m1!1e3!4m6!3m5!1s0x8838594eee81e151:0x7e8393e68e982a37!8m2!3d40.0822196!4d-82.810829!16s%2Fg%2F11px9wd66y?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N30" s="57" t="n"/>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Barn/@40.0632667,-83.1311176,17z/data=!3m2!4b1!5s0x883893a9eb3b54fb:0x949d07058b67c8d5!4m6!3m5!1s0x883893a95e42d91f:0x588486838adf6928!8m2!3d40.0632626!4d-83.1285373!16s%2Fg%2F1tjt2lrl?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Barn/@40.0632626,-83.1285373,548m/data=!3m3!1e3!4b1!5s0x883893a9eb3b54fb:0x949d07058b67c8d5!4m6!3m5!1s0x883893a95e42d91f:0x588486838adf6928!8m2!3d40.0632626!4d-83.1285373!16s%2Fg%2F1tjt2lrl?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U30" s="57" t="n"/>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Saucy+Brew+Works+-+Columbus/@39.9838158,-83.0195792,17z/data=!3m2!4b1!5s0x88388ee7aa146b73:0xcaf6f4a62ccded0e!4m6!3m5!1s0x88388f6efb8530ad:0xb272da1027952abb!8m2!3d39.9838117!4d-83.0169989!16s%2Fg%2F11fwj9l2s9?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Saucy+Brew+Works+Columbus+-+Brewpub+%26+Coffeehouse/@39.9838117,-83.0169989,1097m/data=!3m3!1e3!4b1!5s0x88388ee7aa146b73:0xcaf6f4a62ccded0e!4m6!3m5!1s0x88388f6efb8530ad:0xb272da1027952abb!8m2!3d39.9838117!4d-83.0169989!16s%2Fg%2F11fwj9l2s9?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB30" s="57" t="n"/>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572064,-83.0149452,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572023,-83.0123703,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N31" s="57" t="n"/>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Lucky's+Grille+%26+Sports+Pub/@40.0028286,-83.1535654,17z/data=!3m1!4b1!4m6!3m5!1s0x88389138f184dc67:0xa418d6c3d770177e!8m2!3d40.0028245!4d-83.1509851!16s%2Fg%2F1tffvls3?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Lucky's+Grille+%26+Sports+Pub/@40.0028245,-83.1509851,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389138f184dc67:0xa418d6c3d770177e!8m2!3d40.0028245!4d-83.1509851!16s%2Fg%2F1tffvls3?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U31" s="57" t="n"/>
@@ -4952,7 +4952,7 @@
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Slammies+on+High/@39.9838158,-83.0195792,17z/data=!4m6!3m5!1s0x88388f72863b8b45:0x8afd071c0ccbc293!8m2!3d39.9948991!4d-83.0072908!16s%2Fg%2F11k3jcxth7?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place//@39.9838158,-83.0195792,548m/data=!3m1!1e3?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB31" s="57" t="n"/>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+DogTap+Columbus/@39.8472169,-82.8283464,2094m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387c046920cb17:0x34d1b5c4decdb9ee!8m2!3d39.8472128!4d-82.8257715!16s%2Fg%2F11c4b9y43m?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/BrewDog+DogTap+Columbus/@39.8472128,-82.8257715,550m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387c046920cb17:0x34d1b5c4decdb9ee!8m2!3d39.8472128!4d-82.8257715!16s%2Fg%2F11c4b9y43m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N32" s="57" t="n"/>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.1234821,-82.9837101,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f490ed9d9f63:0x62e80188ea19bc64!8m2!3d40.123478!4d-82.9811298!16s%2Fg%2F1tfjrcf6?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+%26+Grill/@40.123478,-82.9811298,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f490ed9d9f63:0x62e80188ea19bc64!8m2!3d40.123478!4d-82.9811298!16s%2Fg%2F1tfjrcf6?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U32" s="57" t="n"/>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Eupouria+Bar+%26+Patio/@39.9949032,-83.0098711,17z/data=!3m1!5s0x88388ec7d116125d:0x12afa4b7f89fb6a!4m6!3m5!1s0x88388f609b8d94bf:0x34bb3d7b4247c92b!8m2!3d39.9941307!4d-83.0062601!16s%2Fg%2F11vd3v496s?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Eupouria+Bar+%26+Patio/@39.9949032,-83.0098711,548m/data=!3m2!1e3!5s0x88388ec7d116125d:0x12afa4b7f89fb6a!4m6!3m5!1s0x88388f609b8d94bf:0x34bb3d7b4247c92b!8m2!3d39.9941307!4d-83.0062601!16s%2Fg%2F11vd3v496s?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB32" s="57" t="n"/>
@@ -5098,7 +5098,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Double+Eagle+Spirits+%26+Sports/@40.0896138,-83.0531019,1011m/data=!3m1!1e3!4m6!3m5!1s0x88388d35548580cf:0x339b115b62e48f04!8m2!3d40.0896138!4d-83.050527!16s%2Fg%2F11y8lgn94_?entry=tts&amp;g_ep=EgoyMDI1MDIwNS4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Double+Eagle+Spirits+%26+Sports/@40.0896138,-83.0531019,1095m/data=!3m1!1e3!4m6!3m5!1s0x88388d35548580cf:0x339b115b62e48f04!8m2!3d40.0896138!4d-83.050527!16s%2Fg%2F11y8lgn94_?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N33" s="57" t="n"/>
@@ -5123,7 +5123,7 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Draft+Room/@40.1218907,-83.0388852,13.15z/data=!4m6!3m5!1s0x8838f52171949c77:0x6ef99bfabccd0e0b!8m2!3d40.1115192!4d-82.9457222!16s%2Fg%2F11fy_59s1s?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Draft+Room/@40.1218907,-83.0388852,8758m/data=!3m1!1e3!4m6!3m5!1s0x8838f52171949c77:0x6ef99bfabccd0e0b!8m2!3d40.1115192!4d-82.9457222!16s%2Fg%2F11fy_59s1s?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U33" s="57" t="n"/>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Old+North+Arcade+Bar/@40.0151306,-83.0142448,17z/data=!3m1!4b1!4m6!3m5!1s0x88388ea0f5eb8f5f:0x7461da7c108370a9!8m2!3d40.0151265!4d-83.0116645!16s%2Fg%2F11b7015lf2?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Old+North+Arcade+Bar/@40.0151265,-83.0116645,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ea0f5eb8f5f:0x7461da7c108370a9!8m2!3d40.0151265!4d-83.0116645!16s%2Fg%2F11b7015lf2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB33" s="57" t="n"/>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ill+Mannered+Brewing+Company/@40.1633986,-83.0759814,1042m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f20b4ac494e7:0xc620da955e03969e!8m2!3d40.1633945!4d-83.0734065!16s%2Fg%2F11bccm2y3k?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Ill+Mannered+Brewing+Company/@40.1633945,-83.0734065,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f20b4ac494e7:0xc620da955e03969e!8m2!3d40.1633945!4d-83.0734065!16s%2Fg%2F11bccm2y3k?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N34" s="57" t="n"/>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Eastside+Brewing+Co./@39.954109,-82.8080452,17z/data=!3m1!4b1!4m6!3m5!1s0x883865e19a9423bd:0x977444b2c47d068!8m2!3d39.9541049!4d-82.8054649!16s%2Fg%2F11j0qh2tz1?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Eastside+Brewing+Co./@39.9541049,-82.8054649,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883865e19a9423bd:0x977444b2c47d068!8m2!3d39.9541049!4d-82.8054649!16s%2Fg%2F11j0qh2tz1?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U34" s="57" t="n"/>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Upper+Deck/@39.8804438,-83.0731598,17z/data=!3m2!4b1!5s0x883884c8e4a6f543:0x42df2eae4f858b8c!4m6!3m5!1s0x883885d26ff64de3:0x7f7e8e03e8731215!8m2!3d39.8804397!4d-83.0705795!16s%2Fg%2F11h9mvyc84?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Upper+Deck/@39.8804397,-83.0705795,549m/data=!3m3!1e3!4b1!5s0x883884c8e4a6f543:0x42df2eae4f858b8c!4m6!3m5!1s0x883885d26ff64de3:0x7f7e8e03e8731215!8m2!3d39.8804397!4d-83.0705795!16s%2Fg%2F11h9mvyc84?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB34" s="57" t="n"/>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beer+Barrel+Pizza+%26+Grill/@40.108439,-83.1948739,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883895231b161e17:0xd2cf106bfe4ce410!8m2!3d40.1084349!4d-83.192299!16s%2Fg%2F11h53w_d3x?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Beer+Barrel+Pizza+%26+Grill/@40.1084349,-83.192299,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883895231b161e17:0xd2cf106bfe4ce410!8m2!3d40.1084349!4d-83.192299!16s%2Fg%2F11h53w_d3x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N35" s="57" t="n"/>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ill+Mannered+Brewing+Co.+-+Uptown+Marysville/@40.235937,-83.3697476,17z/data=!3m1!4b1!4m6!3m5!1s0x8838c58e20672bc5:0x84d67ad4942ebfa5!8m2!3d40.2359329!4d-83.3671673!16s%2Fg%2F11v5fczx0s?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Ill+Mannered+Brewing+Co.+-+Uptown+Marysville/@40.2359329,-83.3671673,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838c58e20672bc5:0x84d67ad4942ebfa5!8m2!3d40.2359329!4d-83.3671673!16s%2Fg%2F11v5fczx0s?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U35" s="57" t="n"/>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pastimes+Pub+at+Grandview+Yard/@39.9747759,-83.0288768,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f616419a2bf:0x6e58cecfe2b5dfde!8m2!3d39.9747718!4d-83.0262965!16s%2Fg%2F11vlc5j42k?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Pastimes+Pub+at+Grandview+Yard/@39.9747718,-83.0262965,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f616419a2bf:0x6e58cecfe2b5dfde!8m2!3d39.9747718!4d-83.0262965!16s%2Fg%2F11vlc5j42k?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB35" s="57" t="n"/>
@@ -5396,7 +5396,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Cuzn'z+Bar+and+Grill/@39.9563171,-82.7282339,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88386f825f15f403:0x71291ae0b2b07471!8m2!3d39.956313!4d-82.725659!16s%2Fg%2F11byfvy8hx?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Cuzn'z+Bar+and+Grill/@39.956313,-82.725659,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88386f825f15f403:0x71291ae0b2b07471!8m2!3d39.956313!4d-82.725659!16s%2Fg%2F11byfvy8hx?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N36" s="57" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Loose+Rail+Brewing/@39.8432622,-82.8095877,1047m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387be3ae072d43:0x52bb8cac97811b34!8m2!3d39.8432581!4d-82.8070128!16s%2Fg%2F11cssq40xw?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Loose+Rail+Brewing/@39.8432581,-82.8070128,550m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387be3ae072d43:0x52bb8cac97811b34!8m2!3d39.8432581!4d-82.8070128!16s%2Fg%2F11cssq40xw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U36" s="57" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Somewhere+In+Particular+Brewing/@40.0619394,-83.0780191,16z/data=!3m1!4b1!4m6!3m5!1s0x88388d6ffd4f2321:0x9838eefa2e42053b!8m2!3d40.0619353!4d-83.0754388!16s%2Fg%2F11f5k1y058?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Somewhere+In+Particular+Brewing/@40.0619353,-83.0754388,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d6ffd4f2321:0x9838eefa2e42053b!8m2!3d40.0619353!4d-83.0754388!16s%2Fg%2F11f5k1y058?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB36" s="57" t="n"/>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Fattey+Beer+Co./@40.1238795,-82.9336131,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f5436488ec93:0xe7e38bebcbb799e4!8m2!3d40.1238754!4d-82.9310382!16s%2Fg%2F11s4srmvh4?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Fattey+Beer+Co./@40.1238754,-82.9310382,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f5436488ec93:0xe7e38bebcbb799e4!8m2!3d40.1238754!4d-82.9310382!16s%2Fg%2F11s4srmvh4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N37" s="57" t="n"/>
@@ -5523,7 +5523,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Oddfellows+Liquor+Bar/@39.9905766,-83.0152544,17z/data=!4m6!3m5!1s0x88388eda8f91bec7:0x4e305760ecaaefcb!8m2!3d39.9835693!4d-83.0046243!16s%2Fg%2F11b6bv1zr1?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Oddfellows+Liquor+Bar/@39.9905766,-83.0152544,548m/data=!3m1!1e3!4m6!3m5!1s0x88388eda8f91bec7:0x4e305760ecaaefcb!8m2!3d39.9835693!4d-83.0046243!16s%2Fg%2F11b6bv1zr1?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U37" s="57" t="n"/>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1053m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1098m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB37" s="57" t="n"/>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Grainery/@40.1081062,-83.2701861,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838bf0ba726df29:0x3db1fb8e2524cc57!8m2!3d40.1081021!4d-83.2676112!16s%2Fg%2F11h4y5t5yy?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Grainery/@40.1081021,-83.2676112,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838bf0ba726df29:0x3db1fb8e2524cc57!8m2!3d40.1081021!4d-83.2676112!16s%2Fg%2F11h4y5t5yy?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N38" s="57" t="n"/>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Over+Time+Sports+Pub/@39.976551,-82.9853284,20623m/data=!3m1!1e3!4m6!3m5!1s0x883894115efa59bb:0x5defef3ef065d59d!8m2!3d40.039151!4d-83.1806008!16s%2Fg%2F1vgw98vw?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Over+Time+Sports+Pub/@39.976551,-82.9853284,35105m/data=!3m1!1e3!4m6!3m5!1s0x883894115efa59bb:0x5defef3ef065d59d!8m2!3d40.0390917!4d-83.1804997!16s%2Fg%2F1vgw98vw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U38" s="57" t="n"/>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Powell+Bar+%26+Grill/@40.1635164,-83.0766799,1064m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f3fb2e764759:0x2c1bde0bcc10f6bd!8m2!3d40.1635123!4d-83.074105!16s%2Fg%2F11mv5w1cf7?entry=tts&amp;g_ep=EgoyMDI0MTIwOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Powell+Bar+%26+Grill/@40.1635123,-83.074105,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f3fb2e764759:0x2c1bde0bcc10f6bd!8m2!3d40.1635123!4d-83.074105!16s%2Fg%2F11mv5w1cf7?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB38" s="57" t="n"/>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Old+Dog+Alehouse+%26+Brewery/@40.2986278,-83.0710527,1040m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838fb6f65c813f5:0x6a9457798e1d3378!8m2!3d40.2986237!4d-83.0684778!16s%2Fg%2F11gmyvrv5x?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Old+Dog+Alehouse+%26+Brewery/@40.2986237,-83.0684778,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838fb6f65c813f5:0x6a9457798e1d3378!8m2!3d40.2986237!4d-83.0684778!16s%2Fg%2F11gmyvrv5x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N39" s="57" t="n"/>
@@ -5715,7 +5715,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ten+Pin+Alley/@40.0235171,-83.1650249,17z/data=!3m1!4b1!4m6!3m5!1s0x88389155a8e4132d:0xba5d4d8a805a4430!8m2!3d40.023513!4d-83.1624446!16s%2Fg%2F1vlzc0kv?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Ten+Pin+Alley/@40.023513,-83.1624446,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389155a8e4132d:0xba5d4d8a805a4430!8m2!3d40.023513!4d-83.1624446!16s%2Fg%2F1vlzc0kv?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U39" s="57" t="n"/>
@@ -5740,7 +5740,7 @@
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Pickerington)/@39.8851739,-82.757401,17z/data=!3m1!4b1!4m6!3m5!1s0x88387a8ce6424db7:0xbae4fda37aa85f27!8m2!3d39.8851698!4d-82.7548207!16s%2Fg%2F11csrr83pc?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Pickerington)/@39.8851698,-82.7548207,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387a8ce6424db7:0xbae4fda37aa85f27!8m2!3d39.8851698!4d-82.7548207!16s%2Fg%2F11csrr83pc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB39" s="57" t="n"/>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.9893291,-83.0555576,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N40" s="57" t="n"/>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Filling+Station+Bar+%26+Grill/@40.1355168,-83.0745082,17z/data=!3m1!4b1!4m6!3m5!1s0x8838f2851e2f17bb:0x6cf49115a62c037e!8m2!3d40.1355127!4d-83.0719279!16s%2Fg%2F1tdk5vmc?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Filling+Station+Bar+%26+Grill/@40.1355127,-83.0719279,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f2851e2f17bb:0x6cf49115a62c037e!8m2!3d40.1355127!4d-83.0719279!16s%2Fg%2F1tdk5vmc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U40" s="57" t="n"/>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Bobcat+Sports+Bar/@39.9795877,-83.0364103,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f8b1d3ff009:0xa4dca0a665e815f6!8m2!3d39.9795836!4d-83.03383!16s%2Fg%2F11k9h02cd_?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Bobcat+Sports+Bar/@39.9795836,-83.03383,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f8b1d3ff009:0xa4dca0a665e815f6!8m2!3d39.9795836!4d-83.03383!16s%2Fg%2F11k9h02cd_?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB40" s="57" t="n"/>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Rumours+Bar/@39.9416676,-82.9861198,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838895a9a3a4363:0x97f62e465b9f3a10!8m2!3d39.9416635!4d-82.9835449!16s%2Fg%2F11sghnwt_9?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Rumours+Bar/@39.9416635,-82.9835449,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838895a9a3a4363:0x97f62e465b9f3a10!8m2!3d39.9416635!4d-82.9835449!16s%2Fg%2F11sghnwt_9?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N41" s="57" t="n"/>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Average+Joe's/@39.9309561,-83.1041296,11.73z/data=!4m6!3m5!1s0x883890d96dbd9a3d:0xe0fe1dd8d01fdcd0!8m2!3d39.9823075!4d-83.1522751!16s%2Fg%2F12hly9hr3?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Average+Joe's/@39.9309561,-83.1041296,35129m/data=!3m1!1e3!4m6!3m5!1s0x883890d96dbd9a3d:0xe0fe1dd8d01fdcd0!8m2!3d39.9823075!4d-83.1522751!16s%2Fg%2F12hly9hr3?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U41" s="57" t="n"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Forge+Tavern/@40.063024,-83.0586607,16z/data=!3m1!4b1!4m6!3m5!1s0x88388daa28bce9ad:0x49e3fc676cbdcdd8!8m2!3d40.0630199!4d-83.0560804!16s%2Fg%2F11h2hj7qyq?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/The+Forge+Tavern/@40.0630199,-83.0560804,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388daa28bce9ad:0x49e3fc676cbdcdd8!8m2!3d40.0630199!4d-83.0560804!16s%2Fg%2F11h2hj7qyq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB41" s="57" t="n"/>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Local+Bar+Short+North/@39.981131,-83.0075728,2090m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eda04e93d09:0x7123ef06f20bb817!8m2!3d39.9811269!4d-83.0049979!16s%2Fg%2F12lkq9vf7?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Local+Bar+Short+North/@39.9811269,-83.0049979,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388eda04e93d09:0x7123ef06f20bb817!8m2!3d39.9811269!4d-83.0049979!16s%2Fg%2F12lkq9vf7?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N42" s="57" t="n"/>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beerhead+Bar+%26+Eatery/@39.9309561,-83.1041296,11.73z/data=!4m6!3m5!1s0x88386148aba0f9b5:0xb3d992262dcc947!8m2!3d40.079262!4d-82.8495811!16s%2Fg%2F11fvpwcbv5?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Beerhead+Bar+%26+Eatery/@39.9309561,-83.1041296,35129m/data=!3m1!1e3!4m6!3m5!1s0x88386148aba0f9b5:0xb3d992262dcc947!8m2!3d40.079262!4d-82.8495811!16s%2Fg%2F11fvpwcbv5?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U42" s="57" t="n"/>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Crooked+Can+Brewing+Co./@40.034705,-83.1628581,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893f992aea19b:0xe1c8c9ece1f3a626!8m2!3d40.0347009!4d-83.1602832!16s%2Fg%2F11h3vc5lms?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Crooked+Can+Brewing+Co./@40.0347009,-83.1602832,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893f992aea19b:0xe1c8c9ece1f3a626!8m2!3d40.0347009!4d-83.1602832!16s%2Fg%2F11h3vc5lms?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N43" s="57" t="n"/>
@@ -6088,7 +6088,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Eldorado's+Bar+Food+%26+Spirits/@40.0635039,-83.021517,17z/data=!3m1!4b1!4m6!3m5!1s0x88388cf3fabe830b:0xa47ab3892b39be0e!8m2!3d40.0634998!4d-83.0189367!16s%2Fg%2F1v27w4rs?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Eldorado's+Bar+Food+%26+Spirits/@40.0634998,-83.0189367,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388cf3fabe830b:0xa47ab3892b39be0e!8m2!3d40.0634998!4d-83.0189367!16s%2Fg%2F1v27w4rs?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U43" s="57" t="n"/>
@@ -6150,7 +6150,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ohio+Brewing+Company+Columbus/@39.9863181,-83.0081128,17z/data=!4m6!3m5!1s0x88388fa97c327d8b:0xde642ec51d68e5ca!8m2!3d39.9814157!4d-82.9934126!16s%2Fg%2F11rqs_93gg?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Ohio+Brewing+Company+Columbus/@39.9863181,-83.0081128,548m/data=!3m1!1e3!4m6!3m5!1s0x88388fa97c327d8b:0xde642ec51d68e5ca!8m2!3d39.9814157!4d-82.9934126!16s%2Fg%2F11rqs_93gg?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N44" s="57" t="n"/>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Firehouse+Tavern/@40.2405464,-82.8345767,12.66z/data=!4m6!3m5!1s0x883859d1fab35b21:0xe96cd53c584e5c77!8m2!3d40.242194!4d-82.858078!16s%2Fg%2F1tg2f4hp?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Firehouse+Tavern/@40.2405464,-82.8345767,17485m/data=!3m1!1e3!4m6!3m5!1s0x883859d1fab35b21:0xe96cd53c584e5c77!8m2!3d40.242194!4d-82.858078!16s%2Fg%2F1tg2f4hp?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U44" s="57" t="n"/>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1053m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hey+Hey+Bar+%26+Grill/@39.9441748,-82.9898283,1098m/data=!3m1!1e3!4m6!3m5!1s0x883888b1f0564dad:0x87da2bbfdc58bd79!8m2!3d39.9441707!4d-82.9872534!16s%2Fg%2F1td434hd?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N45" s="57" t="n"/>
@@ -6253,7 +6253,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Jerome+Village+Bar+%26+Grille/@40.1663423,-83.1911595,17z/data=!3m2!4b1!5s0x8838eb958802f3f5:0x9003f9c5030ca02a!4m6!3m5!1s0x8838eb93cfa770fb:0xb712bf2eec43c6cf!8m2!3d40.1663383!4d-83.186294!16s%2Fg%2F11h111xw58?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Jerome+Village+Bar+%26+Grille/@40.1663383,-83.186294,547m/data=!3m3!1e3!4b1!5s0x8838eb958802f3f5:0x9003f9c5030ca02a!4m6!3m5!1s0x8838eb93cfa770fb:0xb712bf2eec43c6cf!8m2!3d40.1663383!4d-83.186294!16s%2Fg%2F11h111xw58?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U45" s="57" t="n"/>
@@ -6331,7 +6331,7 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Joe's+Pub+%26+Grill/@40.1549399,-83.097308,17z/data=!3m1!4b1!4m6!3m5!1s0x8838ed90b1372af7:0xfecf3cbe4b484126!8m2!3d40.1549358!4d-83.0947277!16s%2Fg%2F11btv698gn?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Joe's+Pub+%26+Grill/@40.1549358,-83.0947277,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838ed90b1372af7:0xfecf3cbe4b484126!8m2!3d40.1549358!4d-83.0947277!16s%2Fg%2F11btv698gn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U46" s="57" t="n"/>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Pointe+Tavern/@39.9951849,-83.0747946,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e239020b455:0x18f58f231ba40a18!8m2!3d39.9951808!4d-83.0722197!16s%2Fg%2F11bttrpvcv?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Pointe+Tavern/@39.9951808,-83.0722197,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e239020b455:0x18f58f231ba40a18!8m2!3d39.9951808!4d-83.0722197!16s%2Fg%2F11bttrpvcv?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N47" s="57" t="n"/>
@@ -6409,7 +6409,7 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/New+Albany+Links+Golf+Club/@40.1010166,-82.7886007,1050m/data=!3m2!1e3!5s0x88385d99a3d7beeb:0x58e9bb56a310ae5!4m6!3m5!1s0x88385d99bb4f8f8f:0x56cdccbad5e6e9f7!8m2!3d40.1010125!4d-82.7860258!16s%2Fg%2F1tq6kr6y?entry=tts&amp;g_ep=EgoyMDI0MTEyNC4xIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/New+Albany+Links+Golf+Club/@40.1010166,-82.7886007,1095m/data=!3m2!1e3!5s0x88385d99a3d7beeb:0x58e9bb56a310ae5!4m6!3m5!1s0x88385d99bb4f8f8f:0x56cdccbad5e6e9f7!8m2!3d40.1010125!4d-82.7860258!16s%2Fg%2F1tq6kr6y?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U47" s="57" t="n"/>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Parsons+North+Brewing+Company/@39.9498845,-82.985297,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889fa468b5481:0x43c9b00573da795e!8m2!3d39.9498804!4d-82.9827221!16s%2Fg%2F11g1hlg95h?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Parsons+North+Brewing+Company/@39.9498804,-82.9827221,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889fa468b5481:0x43c9b00573da795e!8m2!3d39.9498804!4d-82.9827221!16s%2Fg%2F11g1hlg95h?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N48" s="57" t="n"/>
@@ -6483,7 +6483,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+Short+North/@39.9863181,-83.0081128,17z/data=!3m1!4b1!4m6!3m5!1s0x88388ec53a33fe95:0x974490f6f707d0e3!8m2!3d39.986314!4d-83.0055325!16s%2Fg%2F11hcw4dg65?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/BrewDog+Short+North/@39.986314,-83.0055325,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec53a33fe95:0x974490f6f707d0e3!8m2!3d39.986314!4d-83.0055325!16s%2Fg%2F11hcw4dg65?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U48" s="57" t="n"/>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Signatures+Mill+Stone+Tavern/@40.0200443,-82.8819516,2089m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883861919351ac09:0xb4d411cf697b2e2a!8m2!3d40.0200402!4d-82.8793767!16s%2Fg%2F1tw_nxxq?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Signatures+Mill+Stone+Tavern/@40.0200402,-82.8793767,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883861919351ac09:0xb4d411cf697b2e2a!8m2!3d40.0200402!4d-82.8793767!16s%2Fg%2F1tw_nxxq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N49" s="57" t="n"/>
@@ -6569,7 +6569,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ohio+Brewing+Company+Columbus/@39.9863181,-83.0081128,17z/data=!4m6!3m5!1s0x88388fa97c327d8b:0xde642ec51d68e5ca!8m2!3d39.9814157!4d-82.9934126!16s%2Fg%2F11rqs_93gg?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Ohio+Brewing+Company+Columbus/@39.9863181,-83.0081128,548m/data=!3m1!1e3!4m6!3m5!1s0x88388fa97c327d8b:0xde642ec51d68e5ca!8m2!3d39.9814157!4d-82.9934126!16s%2Fg%2F11rqs_93gg?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U49" s="57" t="n"/>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Classics+Sports+Bar/@39.9236131,-82.7835602,15z/data=!4m6!3m5!1s0x8838658223132ed1:0x2f726b4279e878dc!8m2!3d39.9236131!4d-82.7835602!16s%2Fg%2F11fj_0gbgj?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MDYwNS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Classics+Sports+Bar/@39.9236131,-82.7835602,2196m/data=!3m1!1e3!4m6!3m5!1s0x8838658223132ed1:0x2f726b4279e878dc!8m2!3d39.9236131!4d-82.7835602!16s%2Fg%2F11fj_0gbgj?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N50" s="57" t="n"/>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Slammers/@39.9658369,-82.9982074,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f2d7502487f:0xb1fea5f6dc7ee8a2!8m2!3d39.9658328!4d-82.9956271!16s%2Fg%2F1td3s4q0?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Slammers/@39.9658328,-82.9956271,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f2d7502487f:0xb1fea5f6dc7ee8a2!8m2!3d39.9658328!4d-82.9956271!16s%2Fg%2F1td3s4q0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U50" s="57" t="n"/>
@@ -6704,7 +6704,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beeline+-+Easton+Town+Center/@40.0547016,-82.9153298,1044m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388b9ccfe097a9:0x3f24a794f4ee786!8m2!3d40.0546975!4d-82.9127549!16s%2Fg%2F11fpj6sh1p?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Beeline+-+Easton+Town+Center/@40.0546975,-82.9127549,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388b9ccfe097a9:0x3f24a794f4ee786!8m2!3d40.0546975!4d-82.9127549!16s%2Fg%2F11fpj6sh1p?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N51" s="57" t="n"/>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Plank's+Bier+Garten/@39.9440156,-82.9994235,17z/data=!3m1!4b1!4m6!3m5!1s0x88388f5277c1b1e1:0x31b7de7e1006d9c0!8m2!3d39.9440115!4d-82.9968432!16s%2Fg%2F1tg5cs6n?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Plank's+Bier+Garten/@39.9440115,-82.9968432,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f5277c1b1e1:0x31b7de7e1006d9c0!8m2!3d39.9440115!4d-82.9968432!16s%2Fg%2F1tg5cs6n?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U51" s="57" t="n"/>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577654,-83.0140063,16z/data=!3m1!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N52" s="57" t="n"/>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Town+Center+Pub/@39.8825392,-83.0955623,17z/data=!3m1!4b1!4m6!3m5!1s0x88389b128f70a889:0x1fca7eb81667fadb!8m2!3d39.8825351!4d-83.092982!16s%2Fg%2F11sh0jw_85?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Town+Center+Pub/@39.8825351,-83.092982,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389b128f70a889:0x1fca7eb81667fadb!8m2!3d39.8825351!4d-83.092982!16s%2Fg%2F11sh0jw_85?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U52" s="57" t="n"/>
@@ -6868,7 +6868,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Saturn's+Sports+Bar+Columbus,+Ohio/@39.9887626,-83.0083182,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f6090f08201:0xefbe36917dc45217!8m2!3d39.9887585!4d-83.0057433!16s%2Fg%2F11y21rrkk9?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Saturn's+Sports+Bar+Columbus,+Ohio/@39.9886827,-83.0055231,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f6090f08201:0xefbe36917dc45217!8m2!3d39.9886827!4d-83.0055231!16s%2Fg%2F11y21rrkk9?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N53" s="57" t="n"/>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Tino's+Bar+%26+Grille/@40.1043648,-83.0982116,2068m/data=!3m1!1e3!4m6!3m5!1s0x8838ed4c460476c7:0xf36689ee3cd15003!8m2!3d40.1043607!4d-83.0956367!16s%2Fg%2F12606mmkb?entry=tts&amp;g_ep=EgoyMDI1MDEwNy4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Tino's+Bar+%26+Grille/@40.1043648,-83.0982116,2190m/data=!3m1!1e3!4m6!3m5!1s0x8838ed4c460476c7:0xf36689ee3cd15003!8m2!3d40.1043607!4d-83.0956367!16s%2Fg%2F12606mmkb?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U53" s="57" t="n"/>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Shakers+Public+House/@40.1095313,-82.9993176,4172m/data=!3m1!1e3!4m6!3m5!1s0x88389079eecdb667:0x7f94481966bc381c!8m2!3d40.1095313!4d-82.9993176!16s%2Fg%2F11b6xh8bc2?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Shakers+Public+House/@40.1095313,-82.9993176,4380m/data=!3m1!1e3!4m6!3m5!1s0x88389079eecdb667:0x7f94481966bc381c!8m2!3d40.1095313!4d-82.9993176!16s%2Fg%2F11b6xh8bc2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N54" s="57" t="n"/>
@@ -6967,7 +6967,7 @@
       </c>
       <c r="T54" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/U.A.+Pub/@40.0574893,-83.0769287,17z/data=!3m1!4b1!4m6!3m5!1s0x88388d8ed11a1feb:0xe17e03e59566f602!8m2!3d40.0574852!4d-83.0743484!16s%2Fg%2F11tnw80xd5?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/U.A.+Pub/@40.0574852,-83.0743484,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d8ed11a1feb:0xe17e03e59566f602!8m2!3d40.0574852!4d-83.0743484!16s%2Fg%2F11tnw80xd5?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U54" s="57" t="n"/>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Turtle+Creek+Tavern/@40.0699306,-82.8666647,2087m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838608aa2bf850b:0x7d00e03a844c8c80!8m2!3d40.0699265!4d-82.8640898!16s%2Fg%2F1hhwd448v?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Turtle+Creek+Tavern/@40.0699265,-82.8640898,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838608aa2bf850b:0x7d00e03a844c8c80!8m2!3d40.0699265!4d-82.8640898!16s%2Fg%2F1hhwd448v?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N55" s="57" t="n"/>
@@ -7041,7 +7041,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/North+High+Brewing+-+Dublin/@40.1007093,-83.1163482,1043m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893e43cd525c3:0x88dd86b9cd4e78fd!8m2!3d40.1007052!4d-83.1137733!16s%2Fg%2F11jn0bx047?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/North+High+Brewing+-+Dublin/@40.1007052,-83.1137733,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893e43cd525c3:0x88dd86b9cd4e78fd!8m2!3d40.1007052!4d-83.1137733!16s%2Fg%2F11jn0bx047?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U55" s="57" t="n"/>
@@ -7094,7 +7094,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Union+Cafe/@39.9784197,-83.0058847,1045m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ed9faf67403:0x68da4dab2a9de768!8m2!3d39.9784156!4d-83.0033098!16s%2Fg%2F12hnk04w4?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Union+Cafe/@39.9784156,-83.0033098,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ed9faf67403:0x68da4dab2a9de768!8m2!3d39.9784156!4d-83.0033098!16s%2Fg%2F12hnk04w4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N56" s="97" t="n"/>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="T56" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Gatsby's/@40.0209565,-82.8691971,16z/data=!3m1!4b1!4m6!3m5!1s0x8838619c52bb009f:0xfc7eaa8c3eb1dc41!8m2!3d40.0209524!4d-82.8666168!16s%2Fg%2F1tfmjgvw?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Gatsby's/@40.0209524,-82.8666168,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838619c52bb009f:0xfc7eaa8c3eb1dc41!8m2!3d40.0209524!4d-82.8666168!16s%2Fg%2F1tfmjgvw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U56" s="57" t="n"/>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Scoreboard+Pub+%26+Grill/@40.3067397,-83.0917457,17z/data=!3m1!4b1!4m6!3m5!1s0x8838e4d8079ce4e5:0x6cf5d6861f7dbb30!8m2!3d40.3067356!4d-83.0891654!16s%2Fg%2F11g6rkppdc?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Scoreboard+Pub+%26+Grill/@40.3067356,-83.0891654,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838e4d8079ce4e5:0x6cf5d6861f7dbb30!8m2!3d40.3067356!4d-83.0891654!16s%2Fg%2F11g6rkppdc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N57" s="97" t="n"/>
@@ -7201,7 +7201,7 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Wendell's+Pub/@40.1504481,-82.9250068,1064m/data=!3m3!1e3!4b1!5s0x8838f5938e0b22ef:0x2cb1cde36eb03410!4m6!3m5!1s0x8838f593971e6a41:0x60eab3e48587171!8m2!3d40.150444!4d-82.9224319!16s%2Fg%2F113gdr1tc?entry=tts&amp;g_ep=EgoyMDI0MTIwOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Wendell's+Pub/@40.150444,-82.9224319,1094m/data=!3m3!1e3!4b1!5s0x8838f5938e0b22ef:0x2cb1cde36eb03410!4m6!3m5!1s0x8838f593971e6a41:0x60eab3e48587171!8m2!3d40.150444!4d-82.9224319!16s%2Fg%2F113gdr1tc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U57" s="57" t="n"/>
@@ -7250,7 +7250,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Drexel+Theatre/@39.9236131,-82.7835602,4183m/data=!3m1!1e3!4m6!3m5!1s0x88388844c874d149:0xfd9da6b7bf1138d8!8m2!3d39.9573315!4d-82.9386706!16s%2Fg%2F1vl9s4l8?entry=tts&amp;g_ep=EgoyMDI0MTAyOS4wIPu8ASoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Drexel+Theatre/@39.9236131,-82.7835602,4392m/data=!3m1!1e3!4m6!3m5!1s0x88388844c874d149:0xfd9da6b7bf1138d8!8m2!3d39.9573315!4d-82.9386706!16s%2Fg%2F1vl9s4l8?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N58" s="97" t="n"/>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beef+'O'+Brady's/@40.0337878,-83.1828858,2168m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838941bbc4b0f9b:0x91cf243ce43f2894!8m2!3d40.0337837!4d-83.1803109!16s%2Fg%2F1thf96r0?entry=tts&amp;g_ep=EgoyMDI1MDMxOS4yIPu8ASoASAFQAw%3D%3D&amp;skid=6885fbac-d8a0-4a68-95bb-2db70c63154c</t>
+          <t>https://www.google.com/maps/place/Beef+'O'+Brady's/@40.0337837,-83.1803109,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838941bbc4b0f9b:0x91cf243ce43f2894!8m2!3d40.0337837!4d-83.1803109!16s%2Fg%2F1thf96r0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U58" s="57" t="n"/>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Restoration+Brew+Worx/@40.2996066,-83.07052,17z/data=!3m1!4b1!4m6!3m5!1s0x8838fada04355c15:0x76537e077606e712!8m2!3d40.2996025!4d-83.0679397!16s%2Fg%2F11b7xr9g1r?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Restoration+Brew+Worx/@40.2996025,-83.0679397,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838fada04355c15:0x76537e077606e712!8m2!3d40.2996025!4d-83.0679397!16s%2Fg%2F11b7xr9g1r?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U59" s="57" t="n"/>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Grandview+Cafe/@39.9849211,-83.0471426,17z/data=!3m1!4b1!4m6!3m5!1s0x88388e51af3d6033:0x4e9805ce08a9374b!8m2!3d39.984917!4d-83.0445623!16s%2Fg%2F11b774w5qj?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Grandview+Cafe/@39.984917,-83.0445623,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51af3d6033:0x4e9805ce08a9374b!8m2!3d39.984917!4d-83.0445623!16s%2Fg%2F11b774w5qj?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U60" s="57" t="n"/>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="T61" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Caddy's+Delight+Virtual+Golf+Lounge/@39.9849211,-83.0471426,17z/data=!4m6!3m5!1s0x88388e57d491badf:0x9dd1da930c5fe04e!8m2!3d39.9848966!4d-83.0366112!16s%2Fg%2F11bytn31ln?entry=tts&amp;g_ep=EgoyMDI0MDYwMi4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Caddy's+Delight+Virtual+Golf+Lounge/@39.9849211,-83.0471426,548m/data=!3m1!1e3!4m6!3m5!1s0x88388e57d491badf:0x9dd1da930c5fe04e!8m2!3d39.9848966!4d-83.0366112!16s%2Fg%2F11bytn31ln?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U61" s="57" t="n"/>
@@ -7501,7 +7501,7 @@
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Trek+Brewing+Company/@40.0579069,-82.4561677,15z/data=!4m6!3m5!1s0x88381618d67ec35b:0x7a4f50a9a90ec334!8m2!3d40.0579069!4d-82.4561677!16s%2Fg%2F11fy1l864x?sa=X&amp;ved=1t:2428&amp;ictx=111&amp;entry=tts&amp;g_ep=EgoyMDI0MDYxMS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Trek+Brewing+Company/@40.0579069,-82.4561677,2191m/data=!3m1!1e3!4m6!3m5!1s0x88381618d67ec35b:0x7a4f50a9a90ec334!8m2!3d40.0579069!4d-82.4561677!16s%2Fg%2F11fy1l864x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U62" s="57" t="n"/>
@@ -7551,7 +7551,7 @@
       </c>
       <c r="T63" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Homestead+Taproom+%26+Kitchen/@39.8424255,-82.8059641,15z/data=!4m6!3m5!1s0x88387ba2e353ede3:0x3c9b1badcd31ce8d!8m2!3d39.8424255!4d-82.8059641!16s%2Fg%2F11t_m42xfn?entry=tts&amp;g_ep=EgoyMDI0MDYxNS4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Homestead+Taproom+%26+Kitchen/@39.8424255,-82.8059641,2198m/data=!3m1!1e3!4m6!3m5!1s0x88387ba2e353ede3:0x3c9b1badcd31ce8d!8m2!3d39.8424255!4d-82.8059641!16s%2Fg%2F11t_m42xfn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U63" s="57" t="n"/>
@@ -7605,7 +7605,7 @@
       </c>
       <c r="T64" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Nocterra+Brewing+Co.+-+Powell/@40.1596395,-83.0810736,16z/data=!3m1!4b1!4m6!3m5!1s0x8838f2758d4778c9:0xce79a0c56069e5!8m2!3d40.1596354!4d-83.0784933!16s%2Fg%2F11f3w9tkx2?entry=tts&amp;g_ep=EgoyMDI0MDYwMy4wKgBIAVAD</t>
+          <t>https://www.google.com/maps/place/Nocterra+Brewing+Co.+-+Powell/@40.1596354,-83.0784933,1094m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f2758d4778c9:0xce79a0c56069e5!8m2!3d40.1596354!4d-83.0784933!16s%2Fg%2F11f3w9tkx2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U64" s="57" t="n"/>

</xml_diff>

<commit_message>
Increase the update_xl sleep time to 60 seconds
Last increase of sleep time to 20 seconds was not sufficient to extract the precise coordinates of all the bars (ex. Budd Dairy and Euporia's coordinates are slightly off). Increase to a 60 second sleep time should allow for enough time for the exact coordinates to load.
</commit_message>
<xml_diff>
--- a/data/cbus_trivia_list_updated.xlsx
+++ b/data/cbus_trivia_list_updated.xlsx
@@ -1452,7 +1452,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Homefield:+Iconic+Sports+Bar/@39.9845191,-83.0444814,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51a690bf95:0x39701495d80234e7!8m2!3d39.9845191!4d-83.0444814!16s%2Fg%2F11w4399plq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Homefield:+Iconic+Sports+Bar/@39.9845191,-83.0444814,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51a690bf95:0x39701495d80234e7!8m2!3d39.9845191!4d-83.0444814!16s%2Fg%2F11w4399plq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G3" s="10" t="n"/>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/DraftKings+Sports+%26+Social+Columbus/@39.9795387,-83.0038618,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f0c9732fe45:0xe6466571e35a6f76!8m2!3d39.9795387!4d-83.0038618!16s%2Fg%2F11vw_x7zjs?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/DraftKings+Sports+%26+Social+Columbus/@39.9795387,-83.0038618,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f0c9732fe45:0xe6466571e35a6f76!8m2!3d39.9795387!4d-83.0038618!16s%2Fg%2F11vw_x7zjs?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U3" s="10" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Global+Gallery+Coffee+Shop/@40.0341716,-83.0167931,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c3e50bce2e7:0x4fbf24edfdec3f44!8m2!3d40.0341716!4d-83.0167931!16s%2Fg%2F1tf7hb48?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Global+Gallery+Coffee+Shop/@40.0341716,-83.0167931,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c3e50bce2e7:0x4fbf24edfdec3f44!8m2!3d40.0341716!4d-83.0167931!16s%2Fg%2F1tf7hb48?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI6" s="10" t="n"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Byrne's+Pub/@39.9850105,-83.0389207,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e57001288e1:0xd4c15a5f8359744d!8m2!3d39.9850105!4d-83.0389207!16s%2Fg%2F1tdk5vkn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Byrne's+Pub/@39.9850105,-83.0389207,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e57001288e1:0xd4c15a5f8359744d!8m2!3d39.9850105!4d-83.0389207!16s%2Fg%2F1tdk5vkn?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="G9" s="10" t="n"/>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Bada+Bean+Bada+Booze/@39.9804619,-82.9978676,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f67b407c1a9:0x5557be4d7dfac7e7!8m2!3d39.9804619!4d-82.9978676!16s%2Fg%2F11sb_n85p2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Bada+Bean+Bada+Booze/@39.9804619,-82.9978676,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f67b407c1a9:0x5557be4d7dfac7e7!8m2!3d39.9804619!4d-82.9978676!16s%2Fg%2F11sb_n85p2?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N11" s="10" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Rule+3/@39.9030495,-82.7770293,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387b20bf2a71b3:0x357d7f0b307eb309!8m2!3d39.9030495!4d-82.7770293!16s%2Fg%2F1tg_b4ck?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Rule+3/@39.9030495,-82.7770293,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387b20bf2a71b3:0x357d7f0b307eb309!8m2!3d39.9030495!4d-82.7770293!16s%2Fg%2F1tg_b4ck?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB12" s="10" t="n"/>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Zeno's/@39.9840516,-83.015305,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ee783536759:0xc84ea701e7b579ac!8m2!3d39.9840516!4d-83.015305!16s%2Fg%2F1trrdw5w?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Zeno's/@39.9840516,-83.015305,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ee783536759:0xc84ea701e7b579ac!8m2!3d39.9840516!4d-83.015305!16s%2Fg%2F1trrdw5w?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB14" s="10" t="n"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/India+Oak+Grill/@40.0331459,-82.9999542,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c0c5c53c593:0x17c7304ffff74fed!8m2!3d40.0331459!4d-82.9999542!16s%2Fg%2F1xg5tbg0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/India+Oak+Grill/@40.0331459,-82.9999542,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c0c5c53c593:0x17c7304ffff74fed!8m2!3d40.0331459!4d-82.9999542!16s%2Fg%2F1xg5tbg0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N15" s="10" t="n"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Village+Idiot/@39.9916759,-83.0066832,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec661f8920d:0x422300be0b0a8a5d!8m2!3d39.9916759!4d-83.0066832!16s%2Fg%2F1vqthfx8?authuser=0&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Village+Idiot/@39.9916759,-83.0066832,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ec661f8920d:0x422300be0b0a8a5d!8m2!3d39.9916759!4d-83.0066832!16s%2Fg%2F1vqthfx8?authuser=0&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N19" s="10" t="n"/>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Goat+Dublin/@40.0620135,-83.1733999,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838947b7bbbeafb:0x909c13072f12da01!8m2!3d40.0620135!4d-83.1733999!16s%2Fg%2F1tdnfy3x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Goat+Dublin/@40.0620135,-83.1733999,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838947b7bbbeafb:0x909c13072f12da01!8m2!3d40.0620135!4d-83.1733999!16s%2Fg%2F1tdnfy3x?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N20" s="10" t="n"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Clintonville)/@40.0225052,-83.014128,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d4171aff8a3:0x7c54608c8c482af9!8m2!3d40.0225052!4d-83.014128!16s%2Fg%2F11t7d4d5nw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Combustion+Brewery+%26+Taproom+(Clintonville)/@40.0225052,-83.014128,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388d4171aff8a3:0x7c54608c8c482af9!8m2!3d40.0225052!4d-83.014128!16s%2Fg%2F11t7d4d5nw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AI20" s="57" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Echo+Spirits+Distilling+Co./@39.9890068,-83.0327863,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f4b17d3769b:0x336bfaed8059f751!8m2!3d39.9890068!4d-83.0327863!16s%2Fg%2F11h2fwjvnw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Echo+Spirits+Distilling+Co./@39.9890068,-83.0327863,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f4b17d3769b:0x336bfaed8059f751!8m2!3d39.9890068!4d-83.0327863!16s%2Fg%2F11h2fwjvnw?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U21" s="57" t="n"/>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Goat+RiverSouth/@39.9576025,-82.999999,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f368d224e33:0xb8ba98576f622440!8m2!3d39.9576025!4d-82.999999!16s%2Fg%2F11f3xwp6_m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Goat+RiverSouth/@39.9576025,-82.999999,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f368d224e33:0xb8ba98576f622440!8m2!3d39.9576025!4d-82.999999!16s%2Fg%2F11f3xwp6_m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N22" s="57" t="n"/>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Local+Cantina+-+Clintonville/@40.0259009,-83.0140546,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c180bf51e4d:0x1a9689e6396c477e!8m2!3d40.0259009!4d-83.0140546!16s%2Fg%2F11b6pwcz24?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Local+Cantina+-+Clintonville/@40.0259009,-83.0140546,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388c180bf51e4d:0x1a9689e6396c477e!8m2!3d40.0259009!4d-83.0140546!16s%2Fg%2F11b6pwcz24?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U23" s="57" t="n"/>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Mid+City+Garage/@39.9386553,-82.99099,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889771aed801b:0x5b79881f52ce2dc7!8m2!3d39.9386553!4d-82.99099!16s%2Fg%2F11j5k_spt4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Mid+City+Garage/@39.9386553,-82.99099,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883889771aed801b:0x5b79881f52ce2dc7!8m2!3d39.9386553!4d-82.99099!16s%2Fg%2F11j5k_spt4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U24" s="57" t="n"/>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Submarine+House/@40.001123,-83.1560208,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Submarine+House/@40.001123,-83.1560208,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88389137a6878af7:0xcf6741c2a4a1d1b9!8m2!3d40.001123!4d-83.1560208!16s%2Fg%2F1pzt5cmm4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N26" s="57" t="n"/>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hale%E2%80%99s+Ale+%26+Kitchen/@40.0289201,-83.1190345,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838922c607c7b7b:0xd20f77b84f628c6d!8m2!3d40.0289201!4d-83.1190345!16s%2Fg%2F11bbwnn7f0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Hale%E2%80%99s+Ale+%26+Kitchen/@40.0289201,-83.1190345,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838922c607c7b7b:0xd20f77b84f628c6d!8m2!3d40.0289201!4d-83.1190345!16s%2Fg%2F11bbwnn7f0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N27" s="57" t="n"/>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB28" s="57" t="n"/>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB29" s="57" t="n"/>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572023,-83.0123703,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/BrewDog+Franklinton/@39.9572023,-83.0123703,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3fa5ebffff:0xff6adbcee6017384!8m2!3d39.9572023!4d-83.0123703!16s%2Fg%2F11f50t2qlm?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N31" s="57" t="n"/>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/BrewDog+DogTap+Columbus/@39.8472128,-82.8257715,550m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387c046920cb17:0x34d1b5c4decdb9ee!8m2!3d39.8472128!4d-82.8257715!16s%2Fg%2F11c4b9y43m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/BrewDog+DogTap+Columbus/@39.8472128,-82.8257715,1099m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88387c046920cb17:0x34d1b5c4decdb9ee!8m2!3d39.8472128!4d-82.8257715!16s%2Fg%2F11c4b9y43m?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N32" s="57" t="n"/>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Fattey+Beer+Co./@40.1238754,-82.9310382,547m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f5436488ec93:0xe7e38bebcbb799e4!8m2!3d40.1238754!4d-82.9310382!16s%2Fg%2F11s4srmvh4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Fattey+Beer+Co./@40.1238754,-82.9310382,1095m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838f5436488ec93:0xe7e38bebcbb799e4!8m2!3d40.1238754!4d-82.9310382!16s%2Fg%2F11s4srmvh4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N37" s="57" t="n"/>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Red+Door+Tavern/@39.989325,-83.0529827,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e460e2b1b83:0x489d6c55003fa2a3!8m2!3d39.989325!4d-83.0529827!16s%2Fg%2F1wt3p24j?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N40" s="57" t="n"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/The+Forge+Tavern/@40.0630199,-83.0560804,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388daa28bce9ad:0x49e3fc676cbdcdd8!8m2!3d40.0630199!4d-83.0560804!16s%2Fg%2F11h2hj7qyq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/The+Forge+Tavern/@40.0630199,-83.0560804,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388daa28bce9ad:0x49e3fc676cbdcdd8!8m2!3d40.0630199!4d-83.0560804!16s%2Fg%2F11h2hj7qyq?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="AB41" s="57" t="n"/>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Crooked+Can+Brewing+Co./@40.0347009,-83.1602832,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893f992aea19b:0xe1c8c9ece1f3a626!8m2!3d40.0347009!4d-83.1602832!16s%2Fg%2F11h3vc5lms?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Crooked+Can+Brewing+Co./@40.0347009,-83.1602832,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x883893f992aea19b:0xe1c8c9ece1f3a626!8m2!3d40.0347009!4d-83.1602832!16s%2Fg%2F11h3vc5lms?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N43" s="57" t="n"/>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Plank's+Bier+Garten/@39.9440115,-82.9968432,1098m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f5277c1b1e1:0x31b7de7e1006d9c0!8m2!3d39.9440115!4d-82.9968432!16s%2Fg%2F1tg5cs6n?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Plank's+Bier+Garten/@39.9440115,-82.9968432,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f5277c1b1e1:0x31b7de7e1006d9c0!8m2!3d39.9440115!4d-82.9968432!16s%2Fg%2F1tg5cs6n?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U51" s="57" t="n"/>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Land-Grant+Brewing+Company/@39.9577613,-83.011426,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388f3efd89238b:0xc139207386232411!8m2!3d39.9577613!4d-83.011426!16s%2Fg%2F1pzt7t9df?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N52" s="57" t="n"/>
@@ -7094,7 +7094,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Union+Cafe/@39.9784156,-83.0033098,549m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ed9faf67403:0x68da4dab2a9de768!8m2!3d39.9784156!4d-83.0033098!16s%2Fg%2F12hnk04w4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Union+Cafe/@39.9784156,-83.0033098,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388ed9faf67403:0x68da4dab2a9de768!8m2!3d39.9784156!4d-83.0033098!16s%2Fg%2F12hnk04w4?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N56" s="97" t="n"/>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Scoreboard+Pub+%26+Grill/@40.3067356,-83.0891654,546m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838e4d8079ce4e5:0x6cf5d6861f7dbb30!8m2!3d40.3067356!4d-83.0891654!16s%2Fg%2F11g6rkppdc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Scoreboard+Pub+%26+Grill/@40.3067356,-83.0891654,1092m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838e4d8079ce4e5:0x6cf5d6861f7dbb30!8m2!3d40.3067356!4d-83.0891654!16s%2Fg%2F11g6rkppdc?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="N57" s="97" t="n"/>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Beef+'O'+Brady's/@40.0337837,-83.1803109,548m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838941bbc4b0f9b:0x91cf243ce43f2894!8m2!3d40.0337837!4d-83.1803109!16s%2Fg%2F1thf96r0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place/Beef+'O'+Brady's/@40.0337837,-83.1803109,1096m/data=!3m2!1e3!4b1!4m6!3m5!1s0x8838941bbc4b0f9b:0x91cf243ce43f2894!8m2!3d40.0337837!4d-83.1803109!16s%2Fg%2F1thf96r0?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U58" s="57" t="n"/>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Grandview+Cafe/@39.984917,-83.0445623,1097m/data=!3m2!1e3!4b1!4m6!3m5!1s0x88388e51af3d6033:0x4e9805ce08a9374b!8m2!3d39.984917!4d-83.0445623!16s%2Fg%2F11b774w5qj?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
+          <t>https://www.google.com/maps/place//@39.9849211,-83.0471426,1097m/data=!3m2!1e3!4b1?entry=ttu&amp;g_ep=EgoyMDI1MDQzMC4xIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
       <c r="U60" s="57" t="n"/>

</xml_diff>